<commit_message>
Tokenizador y nuevo diseño para el RPU
</commit_message>
<xml_diff>
--- a/desarrollo_rpu.xlsx
+++ b/desarrollo_rpu.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="26529"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="28025"/>
   <workbookPr codeName="ThisWorkbook" defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Bremdows\UNSAAC\SEMESTRE VIII\ARQUITECTURA DE MICROCONTROLADORES Y MICROPROCESADORES\RPU\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\UNSAAC\SEMESTRE VIII\ARQUITECTURA DE MICROPROCESADORES\arquitectura-digital\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{27FE4B3D-D7E3-4EE0-9D6F-6C971B931342}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{1E5823E8-C7C8-41EE-B4F7-E9F43425BC3F}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="11520" yWindow="456" windowWidth="11520" windowHeight="12504" activeTab="2" xr2:uid="{8E82F3E7-134D-474C-9FA7-3A32119CCF80}"/>
+    <workbookView xWindow="14865" yWindow="0" windowWidth="13935" windowHeight="16200" activeTab="2" xr2:uid="{8E82F3E7-134D-474C-9FA7-3A32119CCF80}"/>
   </bookViews>
   <sheets>
     <sheet name="FSM" sheetId="2" r:id="rId1"/>
@@ -1059,18 +1059,30 @@
     <xf numFmtId="0" fontId="1" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment horizontal="left"/>
     </xf>
+    <xf numFmtId="0" fontId="1" fillId="2" borderId="10" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="2" borderId="11" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="13" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
     <xf numFmtId="0" fontId="0" fillId="2" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="2" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="20" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
     <xf numFmtId="0" fontId="0" fillId="2" borderId="24" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="2" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="2" borderId="13" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
     <xf numFmtId="0" fontId="0" fillId="2" borderId="15" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
@@ -1090,18 +1102,6 @@
       <alignment horizontal="center"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="2" borderId="22" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="2" borderId="20" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="2" borderId="2" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="2" borderId="10" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="2" borderId="11" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
@@ -3163,15 +3163,15 @@
       <xdr:twoCellAnchor editAs="oneCell">
         <xdr:from>
           <xdr:col>6</xdr:col>
-          <xdr:colOff>7620</xdr:colOff>
+          <xdr:colOff>9525</xdr:colOff>
           <xdr:row>5</xdr:row>
-          <xdr:rowOff>83820</xdr:rowOff>
+          <xdr:rowOff>85725</xdr:rowOff>
         </xdr:from>
         <xdr:to>
           <xdr:col>6</xdr:col>
-          <xdr:colOff>1356360</xdr:colOff>
+          <xdr:colOff>1352550</xdr:colOff>
           <xdr:row>7</xdr:row>
-          <xdr:rowOff>60960</xdr:rowOff>
+          <xdr:rowOff>57150</xdr:rowOff>
         </xdr:to>
         <xdr:sp macro="" textlink="">
           <xdr:nvSpPr>
@@ -3523,22 +3523,22 @@
       <selection activeCell="N18" sqref="N18"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
+  <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="3.88671875" style="5" customWidth="1"/>
-    <col min="2" max="2" width="3.88671875" customWidth="1"/>
+    <col min="1" max="1" width="3.85546875" style="5" customWidth="1"/>
+    <col min="2" max="2" width="3.85546875" customWidth="1"/>
     <col min="3" max="3" width="5" customWidth="1"/>
-    <col min="4" max="4" width="6.6640625" customWidth="1"/>
-    <col min="5" max="5" width="6.44140625" customWidth="1"/>
-    <col min="6" max="7" width="4.33203125" style="5" customWidth="1"/>
-    <col min="8" max="8" width="6.88671875" customWidth="1"/>
-    <col min="9" max="12" width="5.33203125" customWidth="1"/>
-    <col min="13" max="15" width="7.33203125" customWidth="1"/>
-    <col min="16" max="41" width="11.44140625" style="5"/>
+    <col min="4" max="4" width="6.7109375" customWidth="1"/>
+    <col min="5" max="5" width="6.42578125" customWidth="1"/>
+    <col min="6" max="7" width="4.28515625" style="5" customWidth="1"/>
+    <col min="8" max="8" width="6.85546875" customWidth="1"/>
+    <col min="9" max="12" width="5.28515625" customWidth="1"/>
+    <col min="13" max="15" width="7.28515625" customWidth="1"/>
+    <col min="16" max="41" width="11.42578125" style="5"/>
   </cols>
   <sheetData>
-    <row r="1" spans="2:15" s="5" customFormat="1" ht="15" thickBot="1" x14ac:dyDescent="0.35"/>
-    <row r="2" spans="2:15" s="5" customFormat="1" ht="15" thickBot="1" x14ac:dyDescent="0.35">
+    <row r="1" spans="2:15" s="5" customFormat="1" ht="15.75" thickBot="1" x14ac:dyDescent="0.3"/>
+    <row r="2" spans="2:15" s="5" customFormat="1" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="I2" s="71" t="s">
         <v>7</v>
       </c>
@@ -3548,7 +3548,7 @@
       </c>
       <c r="L2" s="73"/>
     </row>
-    <row r="3" spans="2:15" ht="15" thickBot="1" x14ac:dyDescent="0.35">
+    <row r="3" spans="2:15" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="B3" s="74" t="s">
         <v>4</v>
       </c>
@@ -3576,7 +3576,7 @@
         <v>14</v>
       </c>
     </row>
-    <row r="4" spans="2:15" x14ac:dyDescent="0.3">
+    <row r="4" spans="2:15" x14ac:dyDescent="0.25">
       <c r="B4" s="3" t="s">
         <v>2</v>
       </c>
@@ -3614,7 +3614,7 @@
         <v>11</v>
       </c>
     </row>
-    <row r="5" spans="2:15" x14ac:dyDescent="0.3">
+    <row r="5" spans="2:15" x14ac:dyDescent="0.25">
       <c r="B5" s="1">
         <v>0</v>
       </c>
@@ -3652,7 +3652,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="6" spans="2:15" x14ac:dyDescent="0.3">
+    <row r="6" spans="2:15" x14ac:dyDescent="0.25">
       <c r="B6" s="1">
         <v>0</v>
       </c>
@@ -3690,7 +3690,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="7" spans="2:15" x14ac:dyDescent="0.3">
+    <row r="7" spans="2:15" x14ac:dyDescent="0.25">
       <c r="B7" s="1">
         <v>1</v>
       </c>
@@ -3728,7 +3728,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="8" spans="2:15" x14ac:dyDescent="0.3">
+    <row r="8" spans="2:15" x14ac:dyDescent="0.25">
       <c r="B8" s="1">
         <v>1</v>
       </c>
@@ -3766,7 +3766,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="9" spans="2:15" s="5" customFormat="1" x14ac:dyDescent="0.3">
+    <row r="9" spans="2:15" s="5" customFormat="1" x14ac:dyDescent="0.25">
       <c r="H9" s="6">
         <v>1</v>
       </c>
@@ -3792,7 +3792,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="10" spans="2:15" s="5" customFormat="1" ht="15" thickBot="1" x14ac:dyDescent="0.35">
+    <row r="10" spans="2:15" s="5" customFormat="1" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="H10" s="6">
         <v>1</v>
       </c>
@@ -3818,7 +3818,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="11" spans="2:15" ht="15" thickBot="1" x14ac:dyDescent="0.35">
+    <row r="11" spans="2:15" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="B11" s="74" t="s">
         <v>5</v>
       </c>
@@ -3852,7 +3852,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="12" spans="2:15" x14ac:dyDescent="0.3">
+    <row r="12" spans="2:15" x14ac:dyDescent="0.25">
       <c r="B12" s="3" t="s">
         <v>2</v>
       </c>
@@ -3890,7 +3890,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="13" spans="2:15" x14ac:dyDescent="0.3">
+    <row r="13" spans="2:15" x14ac:dyDescent="0.25">
       <c r="B13" s="1">
         <v>0</v>
       </c>
@@ -3912,7 +3912,7 @@
       <c r="N13" s="5"/>
       <c r="O13" s="5"/>
     </row>
-    <row r="14" spans="2:15" x14ac:dyDescent="0.3">
+    <row r="14" spans="2:15" x14ac:dyDescent="0.25">
       <c r="B14" s="1">
         <v>0</v>
       </c>
@@ -3934,7 +3934,7 @@
       <c r="N14" s="5"/>
       <c r="O14" s="5"/>
     </row>
-    <row r="15" spans="2:15" x14ac:dyDescent="0.3">
+    <row r="15" spans="2:15" x14ac:dyDescent="0.25">
       <c r="B15" s="1">
         <v>1</v>
       </c>
@@ -3956,7 +3956,7 @@
       <c r="N15" s="5"/>
       <c r="O15" s="5"/>
     </row>
-    <row r="16" spans="2:15" x14ac:dyDescent="0.3">
+    <row r="16" spans="2:15" x14ac:dyDescent="0.25">
       <c r="B16" s="1">
         <v>1</v>
       </c>
@@ -3978,12 +3978,12 @@
       <c r="N16" s="5"/>
       <c r="O16" s="5"/>
     </row>
-    <row r="17" s="5" customFormat="1" x14ac:dyDescent="0.3"/>
-    <row r="18" s="5" customFormat="1" x14ac:dyDescent="0.3"/>
-    <row r="19" s="5" customFormat="1" x14ac:dyDescent="0.3"/>
-    <row r="20" s="5" customFormat="1" x14ac:dyDescent="0.3"/>
-    <row r="21" s="5" customFormat="1" x14ac:dyDescent="0.3"/>
-    <row r="22" s="5" customFormat="1" x14ac:dyDescent="0.3"/>
+    <row r="17" s="5" customFormat="1" x14ac:dyDescent="0.25"/>
+    <row r="18" s="5" customFormat="1" x14ac:dyDescent="0.25"/>
+    <row r="19" s="5" customFormat="1" x14ac:dyDescent="0.25"/>
+    <row r="20" s="5" customFormat="1" x14ac:dyDescent="0.25"/>
+    <row r="21" s="5" customFormat="1" x14ac:dyDescent="0.25"/>
+    <row r="22" s="5" customFormat="1" x14ac:dyDescent="0.25"/>
   </sheetData>
   <mergeCells count="8">
     <mergeCell ref="I2:J2"/>
@@ -4009,23 +4009,23 @@
       <selection activeCell="N16" sqref="N16"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
+  <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="3.88671875" style="5" customWidth="1"/>
-    <col min="2" max="2" width="3.88671875" customWidth="1"/>
+    <col min="1" max="1" width="3.85546875" style="5" customWidth="1"/>
+    <col min="2" max="2" width="3.85546875" customWidth="1"/>
     <col min="3" max="3" width="5" customWidth="1"/>
-    <col min="4" max="4" width="6.6640625" customWidth="1"/>
-    <col min="5" max="5" width="6.44140625" customWidth="1"/>
-    <col min="6" max="7" width="4.33203125" style="5" customWidth="1"/>
-    <col min="8" max="8" width="6.88671875" customWidth="1"/>
-    <col min="9" max="12" width="5.33203125" customWidth="1"/>
-    <col min="13" max="13" width="8.88671875" customWidth="1"/>
-    <col min="14" max="15" width="9.44140625" customWidth="1"/>
-    <col min="16" max="41" width="11.44140625" style="5"/>
+    <col min="4" max="4" width="6.7109375" customWidth="1"/>
+    <col min="5" max="5" width="6.42578125" customWidth="1"/>
+    <col min="6" max="7" width="4.28515625" style="5" customWidth="1"/>
+    <col min="8" max="8" width="6.85546875" customWidth="1"/>
+    <col min="9" max="12" width="5.28515625" customWidth="1"/>
+    <col min="13" max="13" width="8.85546875" customWidth="1"/>
+    <col min="14" max="15" width="9.42578125" customWidth="1"/>
+    <col min="16" max="41" width="11.42578125" style="5"/>
   </cols>
   <sheetData>
-    <row r="1" spans="2:15" s="5" customFormat="1" ht="15" thickBot="1" x14ac:dyDescent="0.35"/>
-    <row r="2" spans="2:15" s="5" customFormat="1" ht="15" thickBot="1" x14ac:dyDescent="0.35">
+    <row r="1" spans="2:15" s="5" customFormat="1" ht="15.75" thickBot="1" x14ac:dyDescent="0.3"/>
+    <row r="2" spans="2:15" s="5" customFormat="1" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="I2" s="71" t="s">
         <v>7</v>
       </c>
@@ -4035,7 +4035,7 @@
       </c>
       <c r="L2" s="73"/>
     </row>
-    <row r="3" spans="2:15" ht="15" thickBot="1" x14ac:dyDescent="0.35">
+    <row r="3" spans="2:15" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="B3" s="74" t="s">
         <v>4</v>
       </c>
@@ -4063,7 +4063,7 @@
         <v>18</v>
       </c>
     </row>
-    <row r="4" spans="2:15" x14ac:dyDescent="0.3">
+    <row r="4" spans="2:15" x14ac:dyDescent="0.25">
       <c r="B4" s="3" t="s">
         <v>2</v>
       </c>
@@ -4101,7 +4101,7 @@
         <v>20</v>
       </c>
     </row>
-    <row r="5" spans="2:15" x14ac:dyDescent="0.3">
+    <row r="5" spans="2:15" x14ac:dyDescent="0.25">
       <c r="B5" s="1">
         <v>0</v>
       </c>
@@ -4139,7 +4139,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="6" spans="2:15" x14ac:dyDescent="0.3">
+    <row r="6" spans="2:15" x14ac:dyDescent="0.25">
       <c r="B6" s="1">
         <v>0</v>
       </c>
@@ -4177,7 +4177,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="7" spans="2:15" x14ac:dyDescent="0.3">
+    <row r="7" spans="2:15" x14ac:dyDescent="0.25">
       <c r="B7" s="1">
         <v>1</v>
       </c>
@@ -4215,7 +4215,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="8" spans="2:15" x14ac:dyDescent="0.3">
+    <row r="8" spans="2:15" x14ac:dyDescent="0.25">
       <c r="B8" s="1">
         <v>1</v>
       </c>
@@ -4253,7 +4253,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="9" spans="2:15" s="5" customFormat="1" x14ac:dyDescent="0.3">
+    <row r="9" spans="2:15" s="5" customFormat="1" x14ac:dyDescent="0.25">
       <c r="H9" s="6">
         <v>1</v>
       </c>
@@ -4279,7 +4279,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="10" spans="2:15" s="5" customFormat="1" ht="15" thickBot="1" x14ac:dyDescent="0.35">
+    <row r="10" spans="2:15" s="5" customFormat="1" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="H10" s="6">
         <v>1</v>
       </c>
@@ -4305,7 +4305,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="11" spans="2:15" ht="15" thickBot="1" x14ac:dyDescent="0.35">
+    <row r="11" spans="2:15" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="B11" s="74" t="s">
         <v>5</v>
       </c>
@@ -4339,7 +4339,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="12" spans="2:15" x14ac:dyDescent="0.3">
+    <row r="12" spans="2:15" x14ac:dyDescent="0.25">
       <c r="B12" s="3" t="s">
         <v>2</v>
       </c>
@@ -4377,7 +4377,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="13" spans="2:15" x14ac:dyDescent="0.3">
+    <row r="13" spans="2:15" x14ac:dyDescent="0.25">
       <c r="B13" s="1">
         <v>0</v>
       </c>
@@ -4399,7 +4399,7 @@
       <c r="N13" s="5"/>
       <c r="O13" s="5"/>
     </row>
-    <row r="14" spans="2:15" x14ac:dyDescent="0.3">
+    <row r="14" spans="2:15" x14ac:dyDescent="0.25">
       <c r="B14" s="1">
         <v>0</v>
       </c>
@@ -4423,7 +4423,7 @@
       <c r="N14" s="80"/>
       <c r="O14" s="80"/>
     </row>
-    <row r="15" spans="2:15" x14ac:dyDescent="0.3">
+    <row r="15" spans="2:15" x14ac:dyDescent="0.25">
       <c r="B15" s="1">
         <v>1</v>
       </c>
@@ -4447,7 +4447,7 @@
       <c r="N15" s="80"/>
       <c r="O15" s="80"/>
     </row>
-    <row r="16" spans="2:15" x14ac:dyDescent="0.3">
+    <row r="16" spans="2:15" x14ac:dyDescent="0.25">
       <c r="B16" s="1">
         <v>1</v>
       </c>
@@ -4469,12 +4469,12 @@
       <c r="N16" s="5"/>
       <c r="O16" s="5"/>
     </row>
-    <row r="17" s="5" customFormat="1" x14ac:dyDescent="0.3"/>
-    <row r="18" s="5" customFormat="1" x14ac:dyDescent="0.3"/>
-    <row r="19" s="5" customFormat="1" x14ac:dyDescent="0.3"/>
-    <row r="20" s="5" customFormat="1" x14ac:dyDescent="0.3"/>
-    <row r="21" s="5" customFormat="1" x14ac:dyDescent="0.3"/>
-    <row r="22" s="5" customFormat="1" x14ac:dyDescent="0.3"/>
+    <row r="17" s="5" customFormat="1" x14ac:dyDescent="0.25"/>
+    <row r="18" s="5" customFormat="1" x14ac:dyDescent="0.25"/>
+    <row r="19" s="5" customFormat="1" x14ac:dyDescent="0.25"/>
+    <row r="20" s="5" customFormat="1" x14ac:dyDescent="0.25"/>
+    <row r="21" s="5" customFormat="1" x14ac:dyDescent="0.25"/>
+    <row r="22" s="5" customFormat="1" x14ac:dyDescent="0.25"/>
   </sheetData>
   <mergeCells count="10">
     <mergeCell ref="B11:C11"/>
@@ -4498,27 +4498,27 @@
   <sheetPr codeName="Hoja3"/>
   <dimension ref="A1:AP187"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A25" zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="J33" sqref="J33"/>
+    <sheetView tabSelected="1" topLeftCell="A17" zoomScale="120" zoomScaleNormal="120" workbookViewId="0">
+      <selection activeCell="I35" sqref="I35"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
+  <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="3.88671875" style="5" customWidth="1"/>
-    <col min="2" max="2" width="3.88671875" customWidth="1"/>
+    <col min="1" max="1" width="3.85546875" style="5" customWidth="1"/>
+    <col min="2" max="2" width="3.85546875" customWidth="1"/>
     <col min="3" max="3" width="5" customWidth="1"/>
-    <col min="4" max="4" width="6.6640625" customWidth="1"/>
-    <col min="5" max="5" width="6.44140625" customWidth="1"/>
-    <col min="6" max="7" width="4.33203125" style="5" customWidth="1"/>
-    <col min="8" max="8" width="6.88671875" customWidth="1"/>
-    <col min="9" max="12" width="5.33203125" customWidth="1"/>
-    <col min="13" max="13" width="8.88671875" customWidth="1"/>
-    <col min="14" max="16" width="9.44140625" customWidth="1"/>
-    <col min="17" max="42" width="11.44140625" style="5"/>
+    <col min="4" max="4" width="6.7109375" customWidth="1"/>
+    <col min="5" max="5" width="6.42578125" customWidth="1"/>
+    <col min="6" max="7" width="4.28515625" style="5" customWidth="1"/>
+    <col min="8" max="8" width="6.85546875" customWidth="1"/>
+    <col min="9" max="12" width="5.28515625" customWidth="1"/>
+    <col min="13" max="13" width="8.85546875" customWidth="1"/>
+    <col min="14" max="16" width="9.42578125" customWidth="1"/>
+    <col min="17" max="42" width="11.42578125" style="5"/>
   </cols>
   <sheetData>
-    <row r="1" spans="2:16" s="5" customFormat="1" ht="15" thickBot="1" x14ac:dyDescent="0.35"/>
-    <row r="2" spans="2:16" s="5" customFormat="1" ht="15" thickBot="1" x14ac:dyDescent="0.35">
+    <row r="1" spans="2:16" s="5" customFormat="1" ht="15.75" thickBot="1" x14ac:dyDescent="0.3"/>
+    <row r="2" spans="2:16" s="5" customFormat="1" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="I2" s="71" t="s">
         <v>7</v>
       </c>
@@ -4528,7 +4528,7 @@
       </c>
       <c r="L2" s="73"/>
     </row>
-    <row r="3" spans="2:16" ht="15" thickBot="1" x14ac:dyDescent="0.35">
+    <row r="3" spans="2:16" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="B3" s="74" t="s">
         <v>4</v>
       </c>
@@ -4559,7 +4559,7 @@
         <v>18</v>
       </c>
     </row>
-    <row r="4" spans="2:16" x14ac:dyDescent="0.3">
+    <row r="4" spans="2:16" x14ac:dyDescent="0.25">
       <c r="B4" s="3" t="s">
         <v>2</v>
       </c>
@@ -4600,7 +4600,7 @@
         <v>20</v>
       </c>
     </row>
-    <row r="5" spans="2:16" x14ac:dyDescent="0.3">
+    <row r="5" spans="2:16" x14ac:dyDescent="0.25">
       <c r="B5" s="1">
         <v>0</v>
       </c>
@@ -4641,7 +4641,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="6" spans="2:16" x14ac:dyDescent="0.3">
+    <row r="6" spans="2:16" x14ac:dyDescent="0.25">
       <c r="B6" s="1">
         <v>0</v>
       </c>
@@ -4682,7 +4682,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="7" spans="2:16" x14ac:dyDescent="0.3">
+    <row r="7" spans="2:16" x14ac:dyDescent="0.25">
       <c r="B7" s="1">
         <v>1</v>
       </c>
@@ -4723,7 +4723,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="8" spans="2:16" x14ac:dyDescent="0.3">
+    <row r="8" spans="2:16" x14ac:dyDescent="0.25">
       <c r="B8" s="1">
         <v>1</v>
       </c>
@@ -4764,7 +4764,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="9" spans="2:16" s="5" customFormat="1" x14ac:dyDescent="0.3">
+    <row r="9" spans="2:16" s="5" customFormat="1" x14ac:dyDescent="0.25">
       <c r="H9" s="19">
         <v>1</v>
       </c>
@@ -4793,7 +4793,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="10" spans="2:16" s="5" customFormat="1" ht="15" thickBot="1" x14ac:dyDescent="0.35">
+    <row r="10" spans="2:16" s="5" customFormat="1" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="H10" s="19">
         <v>1</v>
       </c>
@@ -4822,7 +4822,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="11" spans="2:16" ht="15" thickBot="1" x14ac:dyDescent="0.35">
+    <row r="11" spans="2:16" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="B11" s="74" t="s">
         <v>5</v>
       </c>
@@ -4859,7 +4859,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="12" spans="2:16" ht="15" thickBot="1" x14ac:dyDescent="0.35">
+    <row r="12" spans="2:16" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="B12" s="3" t="s">
         <v>2</v>
       </c>
@@ -4900,7 +4900,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="13" spans="2:16" x14ac:dyDescent="0.3">
+    <row r="13" spans="2:16" x14ac:dyDescent="0.25">
       <c r="B13" s="1">
         <v>0</v>
       </c>
@@ -4923,7 +4923,7 @@
       <c r="O13" s="5"/>
       <c r="P13" s="5"/>
     </row>
-    <row r="14" spans="2:16" x14ac:dyDescent="0.3">
+    <row r="14" spans="2:16" x14ac:dyDescent="0.25">
       <c r="B14" s="1">
         <v>0</v>
       </c>
@@ -4952,7 +4952,7 @@
       </c>
       <c r="P14" s="80"/>
     </row>
-    <row r="15" spans="2:16" x14ac:dyDescent="0.3">
+    <row r="15" spans="2:16" x14ac:dyDescent="0.25">
       <c r="B15" s="1">
         <v>1</v>
       </c>
@@ -4981,7 +4981,7 @@
       </c>
       <c r="P15" s="80"/>
     </row>
-    <row r="16" spans="2:16" ht="15" thickBot="1" x14ac:dyDescent="0.35">
+    <row r="16" spans="2:16" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="B16" s="1">
         <v>1</v>
       </c>
@@ -5004,21 +5004,21 @@
       <c r="O16" s="5"/>
       <c r="P16" s="5"/>
     </row>
-    <row r="17" spans="2:16" s="5" customFormat="1" ht="15" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="H17" s="87" t="s">
+    <row r="17" spans="2:16" s="5" customFormat="1" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="H17" s="91" t="s">
         <v>23</v>
       </c>
-      <c r="I17" s="89"/>
-      <c r="J17" s="89"/>
-      <c r="K17" s="89"/>
-      <c r="L17" s="88"/>
-      <c r="M17" s="87" t="s">
+      <c r="I17" s="93"/>
+      <c r="J17" s="93"/>
+      <c r="K17" s="93"/>
+      <c r="L17" s="92"/>
+      <c r="M17" s="91" t="s">
         <v>44</v>
       </c>
-      <c r="N17" s="88"/>
+      <c r="N17" s="92"/>
       <c r="O17" s="29"/>
     </row>
-    <row r="18" spans="2:16" s="5" customFormat="1" ht="15" thickBot="1" x14ac:dyDescent="0.35">
+    <row r="18" spans="2:16" s="5" customFormat="1" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="B18" s="74" t="s">
         <v>52</v>
       </c>
@@ -5027,15 +5027,15 @@
         <v>6</v>
       </c>
       <c r="E18" s="77"/>
-      <c r="H18" s="94" t="s">
+      <c r="H18" s="81" t="s">
         <v>24</v>
       </c>
-      <c r="I18" s="95"/>
-      <c r="J18" s="95"/>
-      <c r="K18" s="95" t="s">
+      <c r="I18" s="82"/>
+      <c r="J18" s="82"/>
+      <c r="K18" s="82" t="s">
         <v>35</v>
       </c>
-      <c r="L18" s="95"/>
+      <c r="L18" s="82"/>
       <c r="M18" s="10" t="s">
         <v>25</v>
       </c>
@@ -5044,7 +5044,7 @@
       </c>
       <c r="O18" s="30"/>
     </row>
-    <row r="19" spans="2:16" s="5" customFormat="1" x14ac:dyDescent="0.3">
+    <row r="19" spans="2:16" s="5" customFormat="1" x14ac:dyDescent="0.25">
       <c r="B19" s="3" t="s">
         <v>2</v>
       </c>
@@ -5057,15 +5057,15 @@
       <c r="E19" s="3" t="s">
         <v>0</v>
       </c>
-      <c r="H19" s="84" t="s">
+      <c r="H19" s="83" t="s">
         <v>30</v>
       </c>
-      <c r="I19" s="81"/>
-      <c r="J19" s="81"/>
-      <c r="K19" s="81" t="s">
+      <c r="I19" s="84"/>
+      <c r="J19" s="84"/>
+      <c r="K19" s="84" t="s">
         <v>31</v>
       </c>
-      <c r="L19" s="81"/>
+      <c r="L19" s="84"/>
       <c r="M19" s="11" t="s">
         <v>39</v>
       </c>
@@ -5074,7 +5074,7 @@
       </c>
       <c r="O19" s="31"/>
     </row>
-    <row r="20" spans="2:16" s="5" customFormat="1" x14ac:dyDescent="0.3">
+    <row r="20" spans="2:16" s="5" customFormat="1" x14ac:dyDescent="0.25">
       <c r="B20" s="1">
         <v>0</v>
       </c>
@@ -5087,15 +5087,15 @@
       <c r="E20" s="2">
         <v>1</v>
       </c>
-      <c r="H20" s="84" t="s">
+      <c r="H20" s="83" t="s">
         <v>32</v>
       </c>
-      <c r="I20" s="81"/>
-      <c r="J20" s="81"/>
-      <c r="K20" s="81" t="s">
+      <c r="I20" s="84"/>
+      <c r="J20" s="84"/>
+      <c r="K20" s="84" t="s">
         <v>33</v>
       </c>
-      <c r="L20" s="81"/>
+      <c r="L20" s="84"/>
       <c r="M20" s="11" t="s">
         <v>37</v>
       </c>
@@ -5104,7 +5104,7 @@
       </c>
       <c r="O20" s="32"/>
     </row>
-    <row r="21" spans="2:16" s="5" customFormat="1" x14ac:dyDescent="0.3">
+    <row r="21" spans="2:16" s="5" customFormat="1" x14ac:dyDescent="0.25">
       <c r="B21" s="1">
         <v>0</v>
       </c>
@@ -5113,15 +5113,15 @@
       </c>
       <c r="D21" s="2"/>
       <c r="E21" s="2"/>
-      <c r="H21" s="84" t="s">
+      <c r="H21" s="83" t="s">
         <v>43</v>
       </c>
-      <c r="I21" s="81"/>
-      <c r="J21" s="81"/>
-      <c r="K21" s="81" t="s">
+      <c r="I21" s="84"/>
+      <c r="J21" s="84"/>
+      <c r="K21" s="84" t="s">
         <v>36</v>
       </c>
-      <c r="L21" s="81"/>
+      <c r="L21" s="84"/>
       <c r="M21" s="11" t="s">
         <v>38</v>
       </c>
@@ -5130,7 +5130,7 @@
       </c>
       <c r="O21" s="32"/>
     </row>
-    <row r="22" spans="2:16" s="5" customFormat="1" x14ac:dyDescent="0.3">
+    <row r="22" spans="2:16" s="5" customFormat="1" x14ac:dyDescent="0.25">
       <c r="B22" s="1">
         <v>1</v>
       </c>
@@ -5139,15 +5139,15 @@
       </c>
       <c r="D22" s="2"/>
       <c r="E22" s="2"/>
-      <c r="H22" s="90" t="s">
+      <c r="H22" s="94" t="s">
         <v>27</v>
       </c>
-      <c r="I22" s="91"/>
-      <c r="J22" s="92"/>
-      <c r="K22" s="93" t="s">
+      <c r="I22" s="95"/>
+      <c r="J22" s="86"/>
+      <c r="K22" s="85" t="s">
         <v>29</v>
       </c>
-      <c r="L22" s="92"/>
+      <c r="L22" s="86"/>
       <c r="M22" s="11" t="s">
         <v>40</v>
       </c>
@@ -5156,7 +5156,7 @@
       </c>
       <c r="O22" s="31"/>
     </row>
-    <row r="23" spans="2:16" s="5" customFormat="1" x14ac:dyDescent="0.3">
+    <row r="23" spans="2:16" s="5" customFormat="1" x14ac:dyDescent="0.25">
       <c r="B23" s="1">
         <v>1</v>
       </c>
@@ -5165,15 +5165,15 @@
       </c>
       <c r="D23" s="2"/>
       <c r="E23" s="2"/>
-      <c r="H23" s="84" t="s">
+      <c r="H23" s="83" t="s">
         <v>28</v>
       </c>
-      <c r="I23" s="81"/>
-      <c r="J23" s="81"/>
-      <c r="K23" s="81" t="s">
+      <c r="I23" s="84"/>
+      <c r="J23" s="84"/>
+      <c r="K23" s="84" t="s">
         <v>26</v>
       </c>
-      <c r="L23" s="81"/>
+      <c r="L23" s="84"/>
       <c r="M23" s="11" t="s">
         <v>41</v>
       </c>
@@ -5182,36 +5182,36 @@
       </c>
       <c r="O23" s="32"/>
     </row>
-    <row r="24" spans="2:16" s="5" customFormat="1" x14ac:dyDescent="0.3">
-      <c r="H24" s="84"/>
-      <c r="I24" s="81"/>
-      <c r="J24" s="81"/>
-      <c r="K24" s="81"/>
-      <c r="L24" s="81"/>
+    <row r="24" spans="2:16" s="5" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="H24" s="83"/>
+      <c r="I24" s="84"/>
+      <c r="J24" s="84"/>
+      <c r="K24" s="84"/>
+      <c r="L24" s="84"/>
       <c r="M24" s="9"/>
       <c r="N24" s="12"/>
       <c r="O24" s="32"/>
     </row>
-    <row r="25" spans="2:16" s="5" customFormat="1" x14ac:dyDescent="0.3">
-      <c r="H25" s="84"/>
-      <c r="I25" s="81"/>
-      <c r="J25" s="81"/>
-      <c r="K25" s="81"/>
-      <c r="L25" s="81"/>
+    <row r="25" spans="2:16" s="5" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="H25" s="83"/>
+      <c r="I25" s="84"/>
+      <c r="J25" s="84"/>
+      <c r="K25" s="84"/>
+      <c r="L25" s="84"/>
       <c r="M25" s="9"/>
       <c r="N25" s="12"/>
       <c r="O25" s="32"/>
     </row>
-    <row r="26" spans="2:16" s="5" customFormat="1" ht="15" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="H26" s="85" t="s">
+    <row r="26" spans="2:16" s="5" customFormat="1" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="H26" s="89" t="s">
         <v>45</v>
       </c>
-      <c r="I26" s="86"/>
-      <c r="J26" s="86"/>
-      <c r="K26" s="86" t="s">
+      <c r="I26" s="90"/>
+      <c r="J26" s="90"/>
+      <c r="K26" s="90" t="s">
         <v>46</v>
       </c>
-      <c r="L26" s="86"/>
+      <c r="L26" s="90"/>
       <c r="M26" s="15" t="s">
         <v>47</v>
       </c>
@@ -5220,31 +5220,31 @@
       </c>
       <c r="O26" s="31"/>
     </row>
-    <row r="27" spans="2:16" s="5" customFormat="1" x14ac:dyDescent="0.3">
-      <c r="B27" s="81" t="s">
+    <row r="27" spans="2:16" s="5" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="B27" s="84" t="s">
         <v>68</v>
       </c>
-      <c r="C27" s="81"/>
-      <c r="D27" s="81"/>
-      <c r="E27" s="81"/>
-      <c r="F27" s="81"/>
-      <c r="G27" s="81"/>
-    </row>
-    <row r="28" spans="2:16" s="5" customFormat="1" x14ac:dyDescent="0.3">
+      <c r="C27" s="84"/>
+      <c r="D27" s="84"/>
+      <c r="E27" s="84"/>
+      <c r="F27" s="84"/>
+      <c r="G27" s="84"/>
+    </row>
+    <row r="28" spans="2:16" s="5" customFormat="1" x14ac:dyDescent="0.25">
       <c r="B28" s="33" t="s">
         <v>69</v>
       </c>
-      <c r="C28" s="81" t="s">
+      <c r="C28" s="84" t="s">
         <v>70</v>
       </c>
-      <c r="D28" s="81"/>
-      <c r="E28" s="81"/>
-      <c r="F28" s="81" t="s">
+      <c r="D28" s="84"/>
+      <c r="E28" s="84"/>
+      <c r="F28" s="84" t="s">
         <v>18</v>
       </c>
-      <c r="G28" s="81"/>
-    </row>
-    <row r="29" spans="2:16" s="5" customFormat="1" x14ac:dyDescent="0.3">
+      <c r="G28" s="84"/>
+    </row>
+    <row r="29" spans="2:16" s="5" customFormat="1" x14ac:dyDescent="0.25">
       <c r="B29" s="69" t="s">
         <v>61</v>
       </c>
@@ -5268,7 +5268,7 @@
       <c r="O29" s="6"/>
       <c r="P29" s="6"/>
     </row>
-    <row r="30" spans="2:16" s="5" customFormat="1" x14ac:dyDescent="0.3">
+    <row r="30" spans="2:16" s="5" customFormat="1" x14ac:dyDescent="0.25">
       <c r="B30" s="33">
         <v>0</v>
       </c>
@@ -5288,7 +5288,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="31" spans="2:16" s="5" customFormat="1" x14ac:dyDescent="0.3">
+    <row r="31" spans="2:16" s="5" customFormat="1" x14ac:dyDescent="0.25">
       <c r="B31" s="33">
         <v>0</v>
       </c>
@@ -5323,7 +5323,7 @@
         <v>76</v>
       </c>
     </row>
-    <row r="32" spans="2:16" s="5" customFormat="1" ht="15" thickBot="1" x14ac:dyDescent="0.35">
+    <row r="32" spans="2:16" s="5" customFormat="1" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="B32" s="33">
         <v>0</v>
       </c>
@@ -5361,7 +5361,7 @@
         <v>75</v>
       </c>
     </row>
-    <row r="33" spans="2:16" s="5" customFormat="1" x14ac:dyDescent="0.3">
+    <row r="33" spans="2:16" s="5" customFormat="1" x14ac:dyDescent="0.25">
       <c r="B33" s="33">
         <v>0</v>
       </c>
@@ -5391,7 +5391,7 @@
       <c r="O33" s="37"/>
       <c r="P33" s="41"/>
     </row>
-    <row r="34" spans="2:16" s="5" customFormat="1" x14ac:dyDescent="0.3">
+    <row r="34" spans="2:16" s="5" customFormat="1" x14ac:dyDescent="0.25">
       <c r="B34" s="33">
         <v>0</v>
       </c>
@@ -5421,7 +5421,7 @@
       <c r="O34" s="6"/>
       <c r="P34" s="12"/>
     </row>
-    <row r="35" spans="2:16" s="5" customFormat="1" x14ac:dyDescent="0.3">
+    <row r="35" spans="2:16" s="5" customFormat="1" x14ac:dyDescent="0.25">
       <c r="B35" s="33">
         <v>0</v>
       </c>
@@ -5459,7 +5459,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="36" spans="2:16" s="5" customFormat="1" ht="15" thickBot="1" x14ac:dyDescent="0.35">
+    <row r="36" spans="2:16" s="5" customFormat="1" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="B36" s="33">
         <v>0</v>
       </c>
@@ -5491,7 +5491,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="37" spans="2:16" s="5" customFormat="1" x14ac:dyDescent="0.3">
+    <row r="37" spans="2:16" s="5" customFormat="1" x14ac:dyDescent="0.25">
       <c r="B37" s="33">
         <v>0</v>
       </c>
@@ -5510,14 +5510,14 @@
       <c r="G37" s="33">
         <v>0</v>
       </c>
-      <c r="M37" s="82" t="s">
+      <c r="M37" s="87" t="s">
         <v>77</v>
       </c>
-      <c r="N37" s="82"/>
-      <c r="O37" s="82"/>
-      <c r="P37" s="82"/>
-    </row>
-    <row r="38" spans="2:16" s="5" customFormat="1" x14ac:dyDescent="0.3">
+      <c r="N37" s="87"/>
+      <c r="O37" s="87"/>
+      <c r="P37" s="87"/>
+    </row>
+    <row r="38" spans="2:16" s="5" customFormat="1" x14ac:dyDescent="0.25">
       <c r="B38" s="33">
         <v>1</v>
       </c>
@@ -5537,7 +5537,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="39" spans="2:16" s="5" customFormat="1" x14ac:dyDescent="0.3">
+    <row r="39" spans="2:16" s="5" customFormat="1" x14ac:dyDescent="0.25">
       <c r="B39" s="33">
         <v>1</v>
       </c>
@@ -5572,7 +5572,7 @@
         <v>76</v>
       </c>
     </row>
-    <row r="40" spans="2:16" s="5" customFormat="1" ht="15" thickBot="1" x14ac:dyDescent="0.35">
+    <row r="40" spans="2:16" s="5" customFormat="1" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="B40" s="33">
         <v>1</v>
       </c>
@@ -5610,7 +5610,7 @@
         <v>75</v>
       </c>
     </row>
-    <row r="41" spans="2:16" s="5" customFormat="1" x14ac:dyDescent="0.3">
+    <row r="41" spans="2:16" s="5" customFormat="1" x14ac:dyDescent="0.25">
       <c r="B41" s="33">
         <v>1</v>
       </c>
@@ -5640,7 +5640,7 @@
       <c r="O41" s="37"/>
       <c r="P41" s="41"/>
     </row>
-    <row r="42" spans="2:16" s="5" customFormat="1" x14ac:dyDescent="0.3">
+    <row r="42" spans="2:16" s="5" customFormat="1" x14ac:dyDescent="0.25">
       <c r="B42" s="33">
         <v>1</v>
       </c>
@@ -5670,7 +5670,7 @@
       <c r="O42" s="6"/>
       <c r="P42" s="12"/>
     </row>
-    <row r="43" spans="2:16" s="5" customFormat="1" x14ac:dyDescent="0.3">
+    <row r="43" spans="2:16" s="5" customFormat="1" x14ac:dyDescent="0.25">
       <c r="B43" s="33">
         <v>1</v>
       </c>
@@ -5708,7 +5708,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="44" spans="2:16" s="5" customFormat="1" ht="15" thickBot="1" x14ac:dyDescent="0.35">
+    <row r="44" spans="2:16" s="5" customFormat="1" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="B44" s="33">
         <v>1</v>
       </c>
@@ -5740,7 +5740,7 @@
       <c r="O44" s="43"/>
       <c r="P44" s="44"/>
     </row>
-    <row r="45" spans="2:16" s="5" customFormat="1" x14ac:dyDescent="0.3">
+    <row r="45" spans="2:16" s="5" customFormat="1" x14ac:dyDescent="0.25">
       <c r="B45" s="33">
         <v>1</v>
       </c>
@@ -5759,184 +5759,159 @@
       <c r="G45" s="39">
         <v>1</v>
       </c>
-      <c r="K45" s="83" t="s">
+      <c r="K45" s="88" t="s">
         <v>78</v>
       </c>
-      <c r="L45" s="83"/>
-      <c r="M45" s="83"/>
-      <c r="N45" s="83"/>
-      <c r="O45" s="83"/>
-      <c r="P45" s="83"/>
-    </row>
-    <row r="46" spans="2:16" s="5" customFormat="1" x14ac:dyDescent="0.3"/>
-    <row r="47" spans="2:16" s="5" customFormat="1" x14ac:dyDescent="0.3"/>
-    <row r="48" spans="2:16" s="5" customFormat="1" x14ac:dyDescent="0.3"/>
-    <row r="49" s="5" customFormat="1" x14ac:dyDescent="0.3"/>
-    <row r="50" s="5" customFormat="1" x14ac:dyDescent="0.3"/>
-    <row r="51" s="5" customFormat="1" x14ac:dyDescent="0.3"/>
-    <row r="52" s="5" customFormat="1" x14ac:dyDescent="0.3"/>
-    <row r="53" s="5" customFormat="1" x14ac:dyDescent="0.3"/>
-    <row r="54" s="5" customFormat="1" x14ac:dyDescent="0.3"/>
-    <row r="55" s="5" customFormat="1" x14ac:dyDescent="0.3"/>
-    <row r="56" s="5" customFormat="1" x14ac:dyDescent="0.3"/>
-    <row r="57" s="5" customFormat="1" x14ac:dyDescent="0.3"/>
-    <row r="58" s="5" customFormat="1" x14ac:dyDescent="0.3"/>
-    <row r="59" s="5" customFormat="1" x14ac:dyDescent="0.3"/>
-    <row r="60" s="5" customFormat="1" x14ac:dyDescent="0.3"/>
-    <row r="61" s="5" customFormat="1" x14ac:dyDescent="0.3"/>
-    <row r="62" s="5" customFormat="1" x14ac:dyDescent="0.3"/>
-    <row r="63" s="5" customFormat="1" x14ac:dyDescent="0.3"/>
-    <row r="64" s="5" customFormat="1" x14ac:dyDescent="0.3"/>
-    <row r="65" s="5" customFormat="1" x14ac:dyDescent="0.3"/>
-    <row r="66" s="5" customFormat="1" x14ac:dyDescent="0.3"/>
-    <row r="67" s="5" customFormat="1" x14ac:dyDescent="0.3"/>
-    <row r="68" s="5" customFormat="1" x14ac:dyDescent="0.3"/>
-    <row r="69" s="5" customFormat="1" x14ac:dyDescent="0.3"/>
-    <row r="70" s="5" customFormat="1" x14ac:dyDescent="0.3"/>
-    <row r="71" s="5" customFormat="1" x14ac:dyDescent="0.3"/>
-    <row r="72" s="5" customFormat="1" x14ac:dyDescent="0.3"/>
-    <row r="73" s="5" customFormat="1" x14ac:dyDescent="0.3"/>
-    <row r="74" s="5" customFormat="1" x14ac:dyDescent="0.3"/>
-    <row r="75" s="5" customFormat="1" x14ac:dyDescent="0.3"/>
-    <row r="76" s="5" customFormat="1" x14ac:dyDescent="0.3"/>
-    <row r="77" s="5" customFormat="1" x14ac:dyDescent="0.3"/>
-    <row r="78" s="5" customFormat="1" x14ac:dyDescent="0.3"/>
-    <row r="79" s="5" customFormat="1" x14ac:dyDescent="0.3"/>
-    <row r="80" s="5" customFormat="1" x14ac:dyDescent="0.3"/>
-    <row r="81" s="5" customFormat="1" x14ac:dyDescent="0.3"/>
-    <row r="82" s="5" customFormat="1" x14ac:dyDescent="0.3"/>
-    <row r="83" s="5" customFormat="1" x14ac:dyDescent="0.3"/>
-    <row r="84" s="5" customFormat="1" x14ac:dyDescent="0.3"/>
-    <row r="85" s="5" customFormat="1" x14ac:dyDescent="0.3"/>
-    <row r="86" s="5" customFormat="1" x14ac:dyDescent="0.3"/>
-    <row r="87" s="5" customFormat="1" x14ac:dyDescent="0.3"/>
-    <row r="88" s="5" customFormat="1" x14ac:dyDescent="0.3"/>
-    <row r="89" s="5" customFormat="1" x14ac:dyDescent="0.3"/>
-    <row r="90" s="5" customFormat="1" x14ac:dyDescent="0.3"/>
-    <row r="91" s="5" customFormat="1" x14ac:dyDescent="0.3"/>
-    <row r="92" s="5" customFormat="1" x14ac:dyDescent="0.3"/>
-    <row r="93" s="5" customFormat="1" x14ac:dyDescent="0.3"/>
-    <row r="94" s="5" customFormat="1" x14ac:dyDescent="0.3"/>
-    <row r="95" s="5" customFormat="1" x14ac:dyDescent="0.3"/>
-    <row r="96" s="5" customFormat="1" x14ac:dyDescent="0.3"/>
-    <row r="97" s="5" customFormat="1" x14ac:dyDescent="0.3"/>
-    <row r="98" s="5" customFormat="1" x14ac:dyDescent="0.3"/>
-    <row r="99" s="5" customFormat="1" x14ac:dyDescent="0.3"/>
-    <row r="100" s="5" customFormat="1" x14ac:dyDescent="0.3"/>
-    <row r="101" s="5" customFormat="1" x14ac:dyDescent="0.3"/>
-    <row r="102" s="5" customFormat="1" x14ac:dyDescent="0.3"/>
-    <row r="103" s="5" customFormat="1" x14ac:dyDescent="0.3"/>
-    <row r="104" s="5" customFormat="1" x14ac:dyDescent="0.3"/>
-    <row r="105" s="5" customFormat="1" x14ac:dyDescent="0.3"/>
-    <row r="106" s="5" customFormat="1" x14ac:dyDescent="0.3"/>
-    <row r="107" s="5" customFormat="1" x14ac:dyDescent="0.3"/>
-    <row r="108" s="5" customFormat="1" x14ac:dyDescent="0.3"/>
-    <row r="109" s="5" customFormat="1" x14ac:dyDescent="0.3"/>
-    <row r="110" s="5" customFormat="1" x14ac:dyDescent="0.3"/>
-    <row r="111" s="5" customFormat="1" x14ac:dyDescent="0.3"/>
-    <row r="112" s="5" customFormat="1" x14ac:dyDescent="0.3"/>
-    <row r="113" s="5" customFormat="1" x14ac:dyDescent="0.3"/>
-    <row r="114" s="5" customFormat="1" x14ac:dyDescent="0.3"/>
-    <row r="115" s="5" customFormat="1" x14ac:dyDescent="0.3"/>
-    <row r="116" s="5" customFormat="1" x14ac:dyDescent="0.3"/>
-    <row r="117" s="5" customFormat="1" x14ac:dyDescent="0.3"/>
-    <row r="118" s="5" customFormat="1" x14ac:dyDescent="0.3"/>
-    <row r="119" s="5" customFormat="1" x14ac:dyDescent="0.3"/>
-    <row r="120" s="5" customFormat="1" x14ac:dyDescent="0.3"/>
-    <row r="121" s="5" customFormat="1" x14ac:dyDescent="0.3"/>
-    <row r="122" s="5" customFormat="1" x14ac:dyDescent="0.3"/>
-    <row r="123" s="5" customFormat="1" x14ac:dyDescent="0.3"/>
-    <row r="124" s="5" customFormat="1" x14ac:dyDescent="0.3"/>
-    <row r="125" s="5" customFormat="1" x14ac:dyDescent="0.3"/>
-    <row r="126" s="5" customFormat="1" x14ac:dyDescent="0.3"/>
-    <row r="127" s="5" customFormat="1" x14ac:dyDescent="0.3"/>
-    <row r="128" s="5" customFormat="1" x14ac:dyDescent="0.3"/>
-    <row r="129" s="5" customFormat="1" x14ac:dyDescent="0.3"/>
-    <row r="130" s="5" customFormat="1" x14ac:dyDescent="0.3"/>
-    <row r="131" s="5" customFormat="1" x14ac:dyDescent="0.3"/>
-    <row r="132" s="5" customFormat="1" x14ac:dyDescent="0.3"/>
-    <row r="133" s="5" customFormat="1" x14ac:dyDescent="0.3"/>
-    <row r="134" s="5" customFormat="1" x14ac:dyDescent="0.3"/>
-    <row r="135" s="5" customFormat="1" x14ac:dyDescent="0.3"/>
-    <row r="136" s="5" customFormat="1" x14ac:dyDescent="0.3"/>
-    <row r="137" s="5" customFormat="1" x14ac:dyDescent="0.3"/>
-    <row r="138" s="5" customFormat="1" x14ac:dyDescent="0.3"/>
-    <row r="139" s="5" customFormat="1" x14ac:dyDescent="0.3"/>
-    <row r="140" s="5" customFormat="1" x14ac:dyDescent="0.3"/>
-    <row r="141" s="5" customFormat="1" x14ac:dyDescent="0.3"/>
-    <row r="142" s="5" customFormat="1" x14ac:dyDescent="0.3"/>
-    <row r="143" s="5" customFormat="1" x14ac:dyDescent="0.3"/>
-    <row r="144" s="5" customFormat="1" x14ac:dyDescent="0.3"/>
-    <row r="145" s="5" customFormat="1" x14ac:dyDescent="0.3"/>
-    <row r="146" s="5" customFormat="1" x14ac:dyDescent="0.3"/>
-    <row r="147" s="5" customFormat="1" x14ac:dyDescent="0.3"/>
-    <row r="148" s="5" customFormat="1" x14ac:dyDescent="0.3"/>
-    <row r="149" s="5" customFormat="1" x14ac:dyDescent="0.3"/>
-    <row r="150" s="5" customFormat="1" x14ac:dyDescent="0.3"/>
-    <row r="151" s="5" customFormat="1" x14ac:dyDescent="0.3"/>
-    <row r="152" s="5" customFormat="1" x14ac:dyDescent="0.3"/>
-    <row r="153" s="5" customFormat="1" x14ac:dyDescent="0.3"/>
-    <row r="154" s="5" customFormat="1" x14ac:dyDescent="0.3"/>
-    <row r="155" s="5" customFormat="1" x14ac:dyDescent="0.3"/>
-    <row r="156" s="5" customFormat="1" x14ac:dyDescent="0.3"/>
-    <row r="157" s="5" customFormat="1" x14ac:dyDescent="0.3"/>
-    <row r="158" s="5" customFormat="1" x14ac:dyDescent="0.3"/>
-    <row r="159" s="5" customFormat="1" x14ac:dyDescent="0.3"/>
-    <row r="160" s="5" customFormat="1" x14ac:dyDescent="0.3"/>
-    <row r="161" s="5" customFormat="1" x14ac:dyDescent="0.3"/>
-    <row r="162" s="5" customFormat="1" x14ac:dyDescent="0.3"/>
-    <row r="163" s="5" customFormat="1" x14ac:dyDescent="0.3"/>
-    <row r="164" s="5" customFormat="1" x14ac:dyDescent="0.3"/>
-    <row r="165" s="5" customFormat="1" x14ac:dyDescent="0.3"/>
-    <row r="166" s="5" customFormat="1" x14ac:dyDescent="0.3"/>
-    <row r="167" s="5" customFormat="1" x14ac:dyDescent="0.3"/>
-    <row r="168" s="5" customFormat="1" x14ac:dyDescent="0.3"/>
-    <row r="169" s="5" customFormat="1" x14ac:dyDescent="0.3"/>
-    <row r="170" s="5" customFormat="1" x14ac:dyDescent="0.3"/>
-    <row r="171" s="5" customFormat="1" x14ac:dyDescent="0.3"/>
-    <row r="172" s="5" customFormat="1" x14ac:dyDescent="0.3"/>
-    <row r="173" s="5" customFormat="1" x14ac:dyDescent="0.3"/>
-    <row r="174" s="5" customFormat="1" x14ac:dyDescent="0.3"/>
-    <row r="175" s="5" customFormat="1" x14ac:dyDescent="0.3"/>
-    <row r="176" s="5" customFormat="1" x14ac:dyDescent="0.3"/>
-    <row r="177" s="5" customFormat="1" x14ac:dyDescent="0.3"/>
-    <row r="178" s="5" customFormat="1" x14ac:dyDescent="0.3"/>
-    <row r="179" s="5" customFormat="1" x14ac:dyDescent="0.3"/>
-    <row r="180" s="5" customFormat="1" x14ac:dyDescent="0.3"/>
-    <row r="181" s="5" customFormat="1" x14ac:dyDescent="0.3"/>
-    <row r="182" s="5" customFormat="1" x14ac:dyDescent="0.3"/>
-    <row r="183" s="5" customFormat="1" x14ac:dyDescent="0.3"/>
-    <row r="184" s="5" customFormat="1" x14ac:dyDescent="0.3"/>
-    <row r="185" s="5" customFormat="1" x14ac:dyDescent="0.3"/>
-    <row r="186" s="5" customFormat="1" x14ac:dyDescent="0.3"/>
-    <row r="187" s="5" customFormat="1" x14ac:dyDescent="0.3"/>
+      <c r="L45" s="88"/>
+      <c r="M45" s="88"/>
+      <c r="N45" s="88"/>
+      <c r="O45" s="88"/>
+      <c r="P45" s="88"/>
+    </row>
+    <row r="46" spans="2:16" s="5" customFormat="1" x14ac:dyDescent="0.25"/>
+    <row r="47" spans="2:16" s="5" customFormat="1" x14ac:dyDescent="0.25"/>
+    <row r="48" spans="2:16" s="5" customFormat="1" x14ac:dyDescent="0.25"/>
+    <row r="49" s="5" customFormat="1" x14ac:dyDescent="0.25"/>
+    <row r="50" s="5" customFormat="1" x14ac:dyDescent="0.25"/>
+    <row r="51" s="5" customFormat="1" x14ac:dyDescent="0.25"/>
+    <row r="52" s="5" customFormat="1" x14ac:dyDescent="0.25"/>
+    <row r="53" s="5" customFormat="1" x14ac:dyDescent="0.25"/>
+    <row r="54" s="5" customFormat="1" x14ac:dyDescent="0.25"/>
+    <row r="55" s="5" customFormat="1" x14ac:dyDescent="0.25"/>
+    <row r="56" s="5" customFormat="1" x14ac:dyDescent="0.25"/>
+    <row r="57" s="5" customFormat="1" x14ac:dyDescent="0.25"/>
+    <row r="58" s="5" customFormat="1" x14ac:dyDescent="0.25"/>
+    <row r="59" s="5" customFormat="1" x14ac:dyDescent="0.25"/>
+    <row r="60" s="5" customFormat="1" x14ac:dyDescent="0.25"/>
+    <row r="61" s="5" customFormat="1" x14ac:dyDescent="0.25"/>
+    <row r="62" s="5" customFormat="1" x14ac:dyDescent="0.25"/>
+    <row r="63" s="5" customFormat="1" x14ac:dyDescent="0.25"/>
+    <row r="64" s="5" customFormat="1" x14ac:dyDescent="0.25"/>
+    <row r="65" s="5" customFormat="1" x14ac:dyDescent="0.25"/>
+    <row r="66" s="5" customFormat="1" x14ac:dyDescent="0.25"/>
+    <row r="67" s="5" customFormat="1" x14ac:dyDescent="0.25"/>
+    <row r="68" s="5" customFormat="1" x14ac:dyDescent="0.25"/>
+    <row r="69" s="5" customFormat="1" x14ac:dyDescent="0.25"/>
+    <row r="70" s="5" customFormat="1" x14ac:dyDescent="0.25"/>
+    <row r="71" s="5" customFormat="1" x14ac:dyDescent="0.25"/>
+    <row r="72" s="5" customFormat="1" x14ac:dyDescent="0.25"/>
+    <row r="73" s="5" customFormat="1" x14ac:dyDescent="0.25"/>
+    <row r="74" s="5" customFormat="1" x14ac:dyDescent="0.25"/>
+    <row r="75" s="5" customFormat="1" x14ac:dyDescent="0.25"/>
+    <row r="76" s="5" customFormat="1" x14ac:dyDescent="0.25"/>
+    <row r="77" s="5" customFormat="1" x14ac:dyDescent="0.25"/>
+    <row r="78" s="5" customFormat="1" x14ac:dyDescent="0.25"/>
+    <row r="79" s="5" customFormat="1" x14ac:dyDescent="0.25"/>
+    <row r="80" s="5" customFormat="1" x14ac:dyDescent="0.25"/>
+    <row r="81" s="5" customFormat="1" x14ac:dyDescent="0.25"/>
+    <row r="82" s="5" customFormat="1" x14ac:dyDescent="0.25"/>
+    <row r="83" s="5" customFormat="1" x14ac:dyDescent="0.25"/>
+    <row r="84" s="5" customFormat="1" x14ac:dyDescent="0.25"/>
+    <row r="85" s="5" customFormat="1" x14ac:dyDescent="0.25"/>
+    <row r="86" s="5" customFormat="1" x14ac:dyDescent="0.25"/>
+    <row r="87" s="5" customFormat="1" x14ac:dyDescent="0.25"/>
+    <row r="88" s="5" customFormat="1" x14ac:dyDescent="0.25"/>
+    <row r="89" s="5" customFormat="1" x14ac:dyDescent="0.25"/>
+    <row r="90" s="5" customFormat="1" x14ac:dyDescent="0.25"/>
+    <row r="91" s="5" customFormat="1" x14ac:dyDescent="0.25"/>
+    <row r="92" s="5" customFormat="1" x14ac:dyDescent="0.25"/>
+    <row r="93" s="5" customFormat="1" x14ac:dyDescent="0.25"/>
+    <row r="94" s="5" customFormat="1" x14ac:dyDescent="0.25"/>
+    <row r="95" s="5" customFormat="1" x14ac:dyDescent="0.25"/>
+    <row r="96" s="5" customFormat="1" x14ac:dyDescent="0.25"/>
+    <row r="97" s="5" customFormat="1" x14ac:dyDescent="0.25"/>
+    <row r="98" s="5" customFormat="1" x14ac:dyDescent="0.25"/>
+    <row r="99" s="5" customFormat="1" x14ac:dyDescent="0.25"/>
+    <row r="100" s="5" customFormat="1" x14ac:dyDescent="0.25"/>
+    <row r="101" s="5" customFormat="1" x14ac:dyDescent="0.25"/>
+    <row r="102" s="5" customFormat="1" x14ac:dyDescent="0.25"/>
+    <row r="103" s="5" customFormat="1" x14ac:dyDescent="0.25"/>
+    <row r="104" s="5" customFormat="1" x14ac:dyDescent="0.25"/>
+    <row r="105" s="5" customFormat="1" x14ac:dyDescent="0.25"/>
+    <row r="106" s="5" customFormat="1" x14ac:dyDescent="0.25"/>
+    <row r="107" s="5" customFormat="1" x14ac:dyDescent="0.25"/>
+    <row r="108" s="5" customFormat="1" x14ac:dyDescent="0.25"/>
+    <row r="109" s="5" customFormat="1" x14ac:dyDescent="0.25"/>
+    <row r="110" s="5" customFormat="1" x14ac:dyDescent="0.25"/>
+    <row r="111" s="5" customFormat="1" x14ac:dyDescent="0.25"/>
+    <row r="112" s="5" customFormat="1" x14ac:dyDescent="0.25"/>
+    <row r="113" s="5" customFormat="1" x14ac:dyDescent="0.25"/>
+    <row r="114" s="5" customFormat="1" x14ac:dyDescent="0.25"/>
+    <row r="115" s="5" customFormat="1" x14ac:dyDescent="0.25"/>
+    <row r="116" s="5" customFormat="1" x14ac:dyDescent="0.25"/>
+    <row r="117" s="5" customFormat="1" x14ac:dyDescent="0.25"/>
+    <row r="118" s="5" customFormat="1" x14ac:dyDescent="0.25"/>
+    <row r="119" s="5" customFormat="1" x14ac:dyDescent="0.25"/>
+    <row r="120" s="5" customFormat="1" x14ac:dyDescent="0.25"/>
+    <row r="121" s="5" customFormat="1" x14ac:dyDescent="0.25"/>
+    <row r="122" s="5" customFormat="1" x14ac:dyDescent="0.25"/>
+    <row r="123" s="5" customFormat="1" x14ac:dyDescent="0.25"/>
+    <row r="124" s="5" customFormat="1" x14ac:dyDescent="0.25"/>
+    <row r="125" s="5" customFormat="1" x14ac:dyDescent="0.25"/>
+    <row r="126" s="5" customFormat="1" x14ac:dyDescent="0.25"/>
+    <row r="127" s="5" customFormat="1" x14ac:dyDescent="0.25"/>
+    <row r="128" s="5" customFormat="1" x14ac:dyDescent="0.25"/>
+    <row r="129" s="5" customFormat="1" x14ac:dyDescent="0.25"/>
+    <row r="130" s="5" customFormat="1" x14ac:dyDescent="0.25"/>
+    <row r="131" s="5" customFormat="1" x14ac:dyDescent="0.25"/>
+    <row r="132" s="5" customFormat="1" x14ac:dyDescent="0.25"/>
+    <row r="133" s="5" customFormat="1" x14ac:dyDescent="0.25"/>
+    <row r="134" s="5" customFormat="1" x14ac:dyDescent="0.25"/>
+    <row r="135" s="5" customFormat="1" x14ac:dyDescent="0.25"/>
+    <row r="136" s="5" customFormat="1" x14ac:dyDescent="0.25"/>
+    <row r="137" s="5" customFormat="1" x14ac:dyDescent="0.25"/>
+    <row r="138" s="5" customFormat="1" x14ac:dyDescent="0.25"/>
+    <row r="139" s="5" customFormat="1" x14ac:dyDescent="0.25"/>
+    <row r="140" s="5" customFormat="1" x14ac:dyDescent="0.25"/>
+    <row r="141" s="5" customFormat="1" x14ac:dyDescent="0.25"/>
+    <row r="142" s="5" customFormat="1" x14ac:dyDescent="0.25"/>
+    <row r="143" s="5" customFormat="1" x14ac:dyDescent="0.25"/>
+    <row r="144" s="5" customFormat="1" x14ac:dyDescent="0.25"/>
+    <row r="145" s="5" customFormat="1" x14ac:dyDescent="0.25"/>
+    <row r="146" s="5" customFormat="1" x14ac:dyDescent="0.25"/>
+    <row r="147" s="5" customFormat="1" x14ac:dyDescent="0.25"/>
+    <row r="148" s="5" customFormat="1" x14ac:dyDescent="0.25"/>
+    <row r="149" s="5" customFormat="1" x14ac:dyDescent="0.25"/>
+    <row r="150" s="5" customFormat="1" x14ac:dyDescent="0.25"/>
+    <row r="151" s="5" customFormat="1" x14ac:dyDescent="0.25"/>
+    <row r="152" s="5" customFormat="1" x14ac:dyDescent="0.25"/>
+    <row r="153" s="5" customFormat="1" x14ac:dyDescent="0.25"/>
+    <row r="154" s="5" customFormat="1" x14ac:dyDescent="0.25"/>
+    <row r="155" s="5" customFormat="1" x14ac:dyDescent="0.25"/>
+    <row r="156" s="5" customFormat="1" x14ac:dyDescent="0.25"/>
+    <row r="157" s="5" customFormat="1" x14ac:dyDescent="0.25"/>
+    <row r="158" s="5" customFormat="1" x14ac:dyDescent="0.25"/>
+    <row r="159" s="5" customFormat="1" x14ac:dyDescent="0.25"/>
+    <row r="160" s="5" customFormat="1" x14ac:dyDescent="0.25"/>
+    <row r="161" s="5" customFormat="1" x14ac:dyDescent="0.25"/>
+    <row r="162" s="5" customFormat="1" x14ac:dyDescent="0.25"/>
+    <row r="163" s="5" customFormat="1" x14ac:dyDescent="0.25"/>
+    <row r="164" s="5" customFormat="1" x14ac:dyDescent="0.25"/>
+    <row r="165" s="5" customFormat="1" x14ac:dyDescent="0.25"/>
+    <row r="166" s="5" customFormat="1" x14ac:dyDescent="0.25"/>
+    <row r="167" s="5" customFormat="1" x14ac:dyDescent="0.25"/>
+    <row r="168" s="5" customFormat="1" x14ac:dyDescent="0.25"/>
+    <row r="169" s="5" customFormat="1" x14ac:dyDescent="0.25"/>
+    <row r="170" s="5" customFormat="1" x14ac:dyDescent="0.25"/>
+    <row r="171" s="5" customFormat="1" x14ac:dyDescent="0.25"/>
+    <row r="172" s="5" customFormat="1" x14ac:dyDescent="0.25"/>
+    <row r="173" s="5" customFormat="1" x14ac:dyDescent="0.25"/>
+    <row r="174" s="5" customFormat="1" x14ac:dyDescent="0.25"/>
+    <row r="175" s="5" customFormat="1" x14ac:dyDescent="0.25"/>
+    <row r="176" s="5" customFormat="1" x14ac:dyDescent="0.25"/>
+    <row r="177" s="5" customFormat="1" x14ac:dyDescent="0.25"/>
+    <row r="178" s="5" customFormat="1" x14ac:dyDescent="0.25"/>
+    <row r="179" s="5" customFormat="1" x14ac:dyDescent="0.25"/>
+    <row r="180" s="5" customFormat="1" x14ac:dyDescent="0.25"/>
+    <row r="181" s="5" customFormat="1" x14ac:dyDescent="0.25"/>
+    <row r="182" s="5" customFormat="1" x14ac:dyDescent="0.25"/>
+    <row r="183" s="5" customFormat="1" x14ac:dyDescent="0.25"/>
+    <row r="184" s="5" customFormat="1" x14ac:dyDescent="0.25"/>
+    <row r="185" s="5" customFormat="1" x14ac:dyDescent="0.25"/>
+    <row r="186" s="5" customFormat="1" x14ac:dyDescent="0.25"/>
+    <row r="187" s="5" customFormat="1" x14ac:dyDescent="0.25"/>
   </sheetData>
   <mergeCells count="41">
-    <mergeCell ref="I2:J2"/>
-    <mergeCell ref="K2:L2"/>
-    <mergeCell ref="B3:C3"/>
-    <mergeCell ref="D3:E3"/>
-    <mergeCell ref="I3:J3"/>
-    <mergeCell ref="K3:L3"/>
-    <mergeCell ref="B11:C11"/>
-    <mergeCell ref="D11:E11"/>
-    <mergeCell ref="H18:J18"/>
-    <mergeCell ref="K18:L18"/>
-    <mergeCell ref="B18:C18"/>
-    <mergeCell ref="D18:E18"/>
-    <mergeCell ref="H14:L14"/>
-    <mergeCell ref="H15:L15"/>
-    <mergeCell ref="H19:J19"/>
-    <mergeCell ref="K19:L19"/>
-    <mergeCell ref="H20:J20"/>
-    <mergeCell ref="K20:L20"/>
-    <mergeCell ref="H21:J21"/>
-    <mergeCell ref="K21:L21"/>
-    <mergeCell ref="K22:L22"/>
-    <mergeCell ref="H23:J23"/>
-    <mergeCell ref="K23:L23"/>
-    <mergeCell ref="H24:J24"/>
-    <mergeCell ref="K24:L24"/>
     <mergeCell ref="C28:E28"/>
     <mergeCell ref="F28:G28"/>
     <mergeCell ref="M37:P37"/>
@@ -5953,6 +5928,31 @@
     <mergeCell ref="M17:N17"/>
     <mergeCell ref="H17:L17"/>
     <mergeCell ref="H22:J22"/>
+    <mergeCell ref="K22:L22"/>
+    <mergeCell ref="H23:J23"/>
+    <mergeCell ref="K23:L23"/>
+    <mergeCell ref="H24:J24"/>
+    <mergeCell ref="K24:L24"/>
+    <mergeCell ref="H19:J19"/>
+    <mergeCell ref="K19:L19"/>
+    <mergeCell ref="H20:J20"/>
+    <mergeCell ref="K20:L20"/>
+    <mergeCell ref="H21:J21"/>
+    <mergeCell ref="K21:L21"/>
+    <mergeCell ref="B11:C11"/>
+    <mergeCell ref="D11:E11"/>
+    <mergeCell ref="H18:J18"/>
+    <mergeCell ref="K18:L18"/>
+    <mergeCell ref="B18:C18"/>
+    <mergeCell ref="D18:E18"/>
+    <mergeCell ref="H14:L14"/>
+    <mergeCell ref="H15:L15"/>
+    <mergeCell ref="I2:J2"/>
+    <mergeCell ref="K2:L2"/>
+    <mergeCell ref="B3:C3"/>
+    <mergeCell ref="D3:E3"/>
+    <mergeCell ref="I3:J3"/>
+    <mergeCell ref="K3:L3"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <drawing r:id="rId1"/>
@@ -5968,55 +5968,55 @@
       <selection activeCell="I13" sqref="I13"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
+  <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
     <col min="1" max="1" width="7" customWidth="1"/>
-    <col min="2" max="4" width="8.44140625" customWidth="1"/>
-    <col min="5" max="6" width="7.5546875" customWidth="1"/>
+    <col min="2" max="4" width="8.42578125" customWidth="1"/>
+    <col min="5" max="6" width="7.5703125" customWidth="1"/>
     <col min="7" max="8" width="10" customWidth="1"/>
-    <col min="9" max="9" width="5.33203125" customWidth="1"/>
-    <col min="10" max="10" width="10.6640625" customWidth="1"/>
-    <col min="11" max="11" width="9.5546875" customWidth="1"/>
-    <col min="12" max="12" width="10.5546875" customWidth="1"/>
-    <col min="13" max="13" width="4.109375" customWidth="1"/>
+    <col min="9" max="9" width="5.28515625" customWidth="1"/>
+    <col min="10" max="10" width="10.7109375" customWidth="1"/>
+    <col min="11" max="11" width="9.5703125" customWidth="1"/>
+    <col min="12" max="12" width="10.5703125" customWidth="1"/>
+    <col min="13" max="13" width="4.140625" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="2:17" ht="15" thickBot="1" x14ac:dyDescent="0.35"/>
-    <row r="2" spans="2:17" ht="15" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="B2" s="87" t="s">
+    <row r="1" spans="2:17" ht="15.75" thickBot="1" x14ac:dyDescent="0.3"/>
+    <row r="2" spans="2:17" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="B2" s="91" t="s">
         <v>82</v>
       </c>
-      <c r="C2" s="89"/>
-      <c r="D2" s="89"/>
-      <c r="E2" s="89"/>
-      <c r="F2" s="88"/>
-      <c r="G2" s="87" t="s">
+      <c r="C2" s="93"/>
+      <c r="D2" s="93"/>
+      <c r="E2" s="93"/>
+      <c r="F2" s="92"/>
+      <c r="G2" s="91" t="s">
         <v>44</v>
       </c>
-      <c r="H2" s="88"/>
+      <c r="H2" s="92"/>
       <c r="J2" s="50" t="s">
         <v>79</v>
       </c>
-      <c r="K2" s="87" t="s">
+      <c r="K2" s="91" t="s">
         <v>81</v>
       </c>
-      <c r="L2" s="88"/>
+      <c r="L2" s="92"/>
       <c r="M2" s="29"/>
       <c r="N2" s="100" t="s">
         <v>44</v>
       </c>
       <c r="O2" s="101"/>
     </row>
-    <row r="3" spans="2:17" x14ac:dyDescent="0.3">
-      <c r="B3" s="94" t="s">
+    <row r="3" spans="2:17" x14ac:dyDescent="0.25">
+      <c r="B3" s="81" t="s">
         <v>24</v>
       </c>
-      <c r="C3" s="95"/>
-      <c r="D3" s="95"/>
-      <c r="E3" s="95" t="s">
+      <c r="C3" s="82"/>
+      <c r="D3" s="82"/>
+      <c r="E3" s="82" t="s">
         <v>35</v>
       </c>
-      <c r="F3" s="95"/>
+      <c r="F3" s="82"/>
       <c r="G3" s="10" t="s">
         <v>25</v>
       </c>
@@ -6038,16 +6038,16 @@
         <v>58</v>
       </c>
     </row>
-    <row r="4" spans="2:17" x14ac:dyDescent="0.3">
-      <c r="B4" s="84" t="s">
+    <row r="4" spans="2:17" x14ac:dyDescent="0.25">
+      <c r="B4" s="83" t="s">
         <v>30</v>
       </c>
-      <c r="C4" s="81"/>
-      <c r="D4" s="81"/>
-      <c r="E4" s="81" t="s">
+      <c r="C4" s="84"/>
+      <c r="D4" s="84"/>
+      <c r="E4" s="84" t="s">
         <v>31</v>
       </c>
-      <c r="F4" s="81"/>
+      <c r="F4" s="84"/>
       <c r="G4" s="11" t="s">
         <v>39</v>
       </c>
@@ -6069,16 +6069,16 @@
         <v>60</v>
       </c>
     </row>
-    <row r="5" spans="2:17" ht="15" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="B5" s="84" t="s">
+    <row r="5" spans="2:17" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="B5" s="83" t="s">
         <v>32</v>
       </c>
-      <c r="C5" s="81"/>
-      <c r="D5" s="81"/>
-      <c r="E5" s="81" t="s">
+      <c r="C5" s="84"/>
+      <c r="D5" s="84"/>
+      <c r="E5" s="84" t="s">
         <v>33</v>
       </c>
-      <c r="F5" s="81"/>
+      <c r="F5" s="84"/>
       <c r="G5" s="11" t="s">
         <v>37</v>
       </c>
@@ -6099,16 +6099,16 @@
       </c>
       <c r="Q5" s="70"/>
     </row>
-    <row r="6" spans="2:17" x14ac:dyDescent="0.3">
-      <c r="B6" s="84" t="s">
+    <row r="6" spans="2:17" x14ac:dyDescent="0.25">
+      <c r="B6" s="83" t="s">
         <v>43</v>
       </c>
-      <c r="C6" s="81"/>
-      <c r="D6" s="81"/>
-      <c r="E6" s="81" t="s">
+      <c r="C6" s="84"/>
+      <c r="D6" s="84"/>
+      <c r="E6" s="84" t="s">
         <v>36</v>
       </c>
-      <c r="F6" s="81"/>
+      <c r="F6" s="84"/>
       <c r="G6" s="11" t="s">
         <v>38</v>
       </c>
@@ -6117,16 +6117,16 @@
       </c>
       <c r="Q6" s="70"/>
     </row>
-    <row r="7" spans="2:17" x14ac:dyDescent="0.3">
-      <c r="B7" s="90" t="s">
+    <row r="7" spans="2:17" x14ac:dyDescent="0.25">
+      <c r="B7" s="94" t="s">
         <v>27</v>
       </c>
-      <c r="C7" s="91"/>
-      <c r="D7" s="92"/>
-      <c r="E7" s="93" t="s">
+      <c r="C7" s="95"/>
+      <c r="D7" s="86"/>
+      <c r="E7" s="85" t="s">
         <v>67</v>
       </c>
-      <c r="F7" s="92"/>
+      <c r="F7" s="86"/>
       <c r="G7" s="11" t="s">
         <v>40</v>
       </c>
@@ -6134,16 +6134,16 @@
         <v>42</v>
       </c>
     </row>
-    <row r="8" spans="2:17" x14ac:dyDescent="0.3">
-      <c r="B8" s="84" t="s">
+    <row r="8" spans="2:17" x14ac:dyDescent="0.25">
+      <c r="B8" s="83" t="s">
         <v>28</v>
       </c>
-      <c r="C8" s="81"/>
-      <c r="D8" s="81"/>
-      <c r="E8" s="81" t="s">
+      <c r="C8" s="84"/>
+      <c r="D8" s="84"/>
+      <c r="E8" s="84" t="s">
         <v>26</v>
       </c>
-      <c r="F8" s="81"/>
+      <c r="F8" s="84"/>
       <c r="G8" s="11" t="s">
         <v>41</v>
       </c>
@@ -6163,12 +6163,12 @@
       </c>
       <c r="O8" s="96"/>
     </row>
-    <row r="9" spans="2:17" x14ac:dyDescent="0.3">
-      <c r="B9" s="84"/>
-      <c r="C9" s="81"/>
-      <c r="D9" s="81"/>
-      <c r="E9" s="81"/>
-      <c r="F9" s="81"/>
+    <row r="9" spans="2:17" x14ac:dyDescent="0.25">
+      <c r="B9" s="83"/>
+      <c r="C9" s="84"/>
+      <c r="D9" s="84"/>
+      <c r="E9" s="84"/>
+      <c r="F9" s="84"/>
       <c r="G9" s="9"/>
       <c r="H9" s="12"/>
       <c r="J9" s="65"/>
@@ -6183,12 +6183,12 @@
         <v>58</v>
       </c>
     </row>
-    <row r="10" spans="2:17" x14ac:dyDescent="0.3">
-      <c r="B10" s="84"/>
-      <c r="C10" s="81"/>
-      <c r="D10" s="81"/>
-      <c r="E10" s="81"/>
-      <c r="F10" s="81"/>
+    <row r="10" spans="2:17" x14ac:dyDescent="0.25">
+      <c r="B10" s="83"/>
+      <c r="C10" s="84"/>
+      <c r="D10" s="84"/>
+      <c r="E10" s="84"/>
+      <c r="F10" s="84"/>
       <c r="G10" s="9"/>
       <c r="H10" s="12"/>
       <c r="J10" s="65"/>
@@ -6205,16 +6205,16 @@
         <v>89</v>
       </c>
     </row>
-    <row r="11" spans="2:17" ht="15" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="B11" s="85" t="s">
+    <row r="11" spans="2:17" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="B11" s="89" t="s">
         <v>45</v>
       </c>
-      <c r="C11" s="86"/>
-      <c r="D11" s="86"/>
-      <c r="E11" s="86" t="s">
+      <c r="C11" s="90"/>
+      <c r="D11" s="90"/>
+      <c r="E11" s="90" t="s">
         <v>46</v>
       </c>
-      <c r="F11" s="86"/>
+      <c r="F11" s="90"/>
       <c r="G11" s="15" t="s">
         <v>47</v>
       </c>
@@ -6233,7 +6233,7 @@
         <v>58</v>
       </c>
     </row>
-    <row r="12" spans="2:17" x14ac:dyDescent="0.3">
+    <row r="12" spans="2:17" x14ac:dyDescent="0.25">
       <c r="J12" s="65"/>
       <c r="K12" s="1" t="s">
         <v>29</v>
@@ -6246,7 +6246,7 @@
         <v>58</v>
       </c>
     </row>
-    <row r="13" spans="2:17" x14ac:dyDescent="0.3">
+    <row r="13" spans="2:17" x14ac:dyDescent="0.25">
       <c r="J13" s="65"/>
       <c r="K13" s="1" t="s">
         <v>26</v>
@@ -6261,6 +6261,15 @@
     </row>
   </sheetData>
   <mergeCells count="25">
+    <mergeCell ref="E6:F6"/>
+    <mergeCell ref="B7:D7"/>
+    <mergeCell ref="E7:F7"/>
+    <mergeCell ref="B2:F2"/>
+    <mergeCell ref="G2:H2"/>
+    <mergeCell ref="B3:D3"/>
+    <mergeCell ref="E3:F3"/>
+    <mergeCell ref="B4:D4"/>
+    <mergeCell ref="E4:F4"/>
     <mergeCell ref="K8:L8"/>
     <mergeCell ref="N8:O8"/>
     <mergeCell ref="J3:J5"/>
@@ -6277,15 +6286,6 @@
     <mergeCell ref="B5:D5"/>
     <mergeCell ref="E5:F5"/>
     <mergeCell ref="B6:D6"/>
-    <mergeCell ref="E6:F6"/>
-    <mergeCell ref="B7:D7"/>
-    <mergeCell ref="E7:F7"/>
-    <mergeCell ref="B2:F2"/>
-    <mergeCell ref="G2:H2"/>
-    <mergeCell ref="B3:D3"/>
-    <mergeCell ref="E3:F3"/>
-    <mergeCell ref="B4:D4"/>
-    <mergeCell ref="E4:F4"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup paperSize="9" orientation="portrait" r:id="rId1"/>
@@ -6301,18 +6301,18 @@
       <selection activeCell="B12" sqref="B12"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
+  <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="11.44140625" style="46"/>
-    <col min="4" max="5" width="11.44140625" style="46"/>
-    <col min="6" max="6" width="3.6640625" customWidth="1"/>
+    <col min="1" max="1" width="11.42578125" style="46"/>
+    <col min="4" max="5" width="11.42578125" style="46"/>
+    <col min="6" max="6" width="3.7109375" customWidth="1"/>
     <col min="7" max="7" width="20" customWidth="1"/>
-    <col min="9" max="9" width="20.109375" customWidth="1"/>
-    <col min="12" max="12" width="10.33203125" customWidth="1"/>
+    <col min="9" max="9" width="20.140625" customWidth="1"/>
+    <col min="12" max="12" width="10.28515625" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:12" ht="15" thickBot="1" x14ac:dyDescent="0.35"/>
-    <row r="2" spans="1:12" ht="18.600000000000001" thickBot="1" x14ac:dyDescent="0.35">
+    <row r="1" spans="1:12" ht="15.75" thickBot="1" x14ac:dyDescent="0.3"/>
+    <row r="2" spans="1:12" ht="19.5" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A2" s="102" t="s">
         <v>87</v>
       </c>
@@ -6323,13 +6323,13 @@
       <c r="F2" s="103"/>
       <c r="G2" s="104"/>
     </row>
-    <row r="3" spans="1:12" ht="15" thickBot="1" x14ac:dyDescent="0.35">
+    <row r="3" spans="1:12" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="B3" s="46"/>
       <c r="C3" s="46"/>
       <c r="F3" s="46"/>
       <c r="G3" s="46"/>
     </row>
-    <row r="4" spans="1:12" ht="15" thickBot="1" x14ac:dyDescent="0.35">
+    <row r="4" spans="1:12" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A4" s="61" t="s">
         <v>83</v>
       </c>
@@ -6349,7 +6349,7 @@
         <v>86</v>
       </c>
     </row>
-    <row r="5" spans="1:12" ht="15" thickBot="1" x14ac:dyDescent="0.35">
+    <row r="5" spans="1:12" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A5" s="1">
         <v>0</v>
       </c>
@@ -6370,16 +6370,16 @@
       <c r="G5" s="63" t="s">
         <v>88</v>
       </c>
-      <c r="I5" s="87" t="s">
+      <c r="I5" s="91" t="s">
         <v>82</v>
       </c>
-      <c r="J5" s="89"/>
-      <c r="K5" s="87" t="s">
+      <c r="J5" s="93"/>
+      <c r="K5" s="91" t="s">
         <v>44</v>
       </c>
-      <c r="L5" s="88"/>
-    </row>
-    <row r="6" spans="1:12" x14ac:dyDescent="0.3">
+      <c r="L5" s="92"/>
+    </row>
+    <row r="6" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A6" s="1">
         <f>A5+1</f>
         <v>1</v>
@@ -6411,7 +6411,7 @@
         <v>34</v>
       </c>
     </row>
-    <row r="7" spans="1:12" x14ac:dyDescent="0.3">
+    <row r="7" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A7" s="1">
         <f t="shared" ref="A7:A24" si="2">A6+1</f>
         <v>2</v>
@@ -6443,7 +6443,7 @@
         <v>42</v>
       </c>
     </row>
-    <row r="8" spans="1:12" x14ac:dyDescent="0.3">
+    <row r="8" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A8" s="1">
         <f t="shared" si="2"/>
         <v>3</v>
@@ -6475,7 +6475,7 @@
         <v>8</v>
       </c>
     </row>
-    <row r="9" spans="1:12" x14ac:dyDescent="0.3">
+    <row r="9" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A9" s="1">
         <f t="shared" si="2"/>
         <v>4</v>
@@ -6507,7 +6507,7 @@
         <v>8</v>
       </c>
     </row>
-    <row r="10" spans="1:12" x14ac:dyDescent="0.3">
+    <row r="10" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A10" s="1">
         <f t="shared" si="2"/>
         <v>5</v>
@@ -6539,7 +6539,7 @@
         <v>42</v>
       </c>
     </row>
-    <row r="11" spans="1:12" x14ac:dyDescent="0.3">
+    <row r="11" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A11" s="1">
         <f t="shared" si="2"/>
         <v>6</v>
@@ -6571,7 +6571,7 @@
         <v>42</v>
       </c>
     </row>
-    <row r="12" spans="1:12" x14ac:dyDescent="0.3">
+    <row r="12" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A12" s="1">
         <f t="shared" si="2"/>
         <v>7</v>
@@ -6595,7 +6595,7 @@
       <c r="K12" s="9"/>
       <c r="L12" s="12"/>
     </row>
-    <row r="13" spans="1:12" x14ac:dyDescent="0.3">
+    <row r="13" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A13" s="1">
         <f t="shared" si="2"/>
         <v>8</v>
@@ -6617,7 +6617,7 @@
       <c r="K13" s="9"/>
       <c r="L13" s="12"/>
     </row>
-    <row r="14" spans="1:12" ht="15" thickBot="1" x14ac:dyDescent="0.35">
+    <row r="14" spans="1:12" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A14" s="1">
         <f t="shared" si="2"/>
         <v>9</v>
@@ -6647,7 +6647,7 @@
         <v>42</v>
       </c>
     </row>
-    <row r="15" spans="1:12" x14ac:dyDescent="0.3">
+    <row r="15" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A15" s="1">
         <f t="shared" si="2"/>
         <v>10</v>
@@ -6665,7 +6665,7 @@
         <v>00000</v>
       </c>
     </row>
-    <row r="16" spans="1:12" x14ac:dyDescent="0.3">
+    <row r="16" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A16" s="1">
         <f t="shared" si="2"/>
         <v>11</v>
@@ -6683,7 +6683,7 @@
         <v>00000</v>
       </c>
     </row>
-    <row r="17" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="17" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A17" s="1">
         <f t="shared" si="2"/>
         <v>12</v>
@@ -6701,7 +6701,7 @@
         <v>00000</v>
       </c>
     </row>
-    <row r="18" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="18" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A18" s="1">
         <f t="shared" si="2"/>
         <v>13</v>
@@ -6719,7 +6719,7 @@
         <v>00000</v>
       </c>
     </row>
-    <row r="19" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="19" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A19" s="1">
         <f t="shared" si="2"/>
         <v>14</v>
@@ -6737,7 +6737,7 @@
         <v>00000</v>
       </c>
     </row>
-    <row r="20" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="20" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A20" s="1">
         <f t="shared" si="2"/>
         <v>15</v>
@@ -6755,7 +6755,7 @@
         <v>00000</v>
       </c>
     </row>
-    <row r="21" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="21" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A21" s="1">
         <f t="shared" si="2"/>
         <v>16</v>
@@ -6773,7 +6773,7 @@
         <v>00000</v>
       </c>
     </row>
-    <row r="22" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="22" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A22" s="1">
         <f t="shared" si="2"/>
         <v>17</v>
@@ -6791,7 +6791,7 @@
         <v>00000</v>
       </c>
     </row>
-    <row r="23" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="23" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A23" s="1">
         <f t="shared" si="2"/>
         <v>18</v>
@@ -6809,7 +6809,7 @@
         <v>00000</v>
       </c>
     </row>
-    <row r="24" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="24" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A24" s="1">
         <f t="shared" si="2"/>
         <v>19</v>
@@ -6849,15 +6849,15 @@
             <anchor moveWithCells="1">
               <from>
                 <xdr:col>6</xdr:col>
-                <xdr:colOff>7620</xdr:colOff>
+                <xdr:colOff>9525</xdr:colOff>
                 <xdr:row>5</xdr:row>
-                <xdr:rowOff>83820</xdr:rowOff>
+                <xdr:rowOff>85725</xdr:rowOff>
               </from>
               <to>
-                <xdr:col>6</xdr:col>
-                <xdr:colOff>1356360</xdr:colOff>
+                <xdr:col>7</xdr:col>
+                <xdr:colOff>28575</xdr:colOff>
                 <xdr:row>7</xdr:row>
-                <xdr:rowOff>60960</xdr:rowOff>
+                <xdr:rowOff>47625</xdr:rowOff>
               </to>
             </anchor>
           </controlPr>
@@ -6880,7 +6880,7 @@
       <selection activeCell="G10" sqref="G10"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
+  <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <sheetData/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>

</xml_diff>

<commit_message>
TA: Arquitectura de Hardware - finalizada
</commit_message>
<xml_diff>
--- a/desarrollo_rpu.xlsx
+++ b/desarrollo_rpu.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="28025"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="26529"/>
   <workbookPr codeName="ThisWorkbook" defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\UNSAAC\SEMESTRE VIII\ARQUITECTURA DE MICROPROCESADORES\arquitectura-digital\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Bremdows\UNSAAC\SEMESTRE VIII\ARQUITECTURA DE MICROCONTROLADORES Y MICROPROCESADORES\arquitectura-digital\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{1E5823E8-C7C8-41EE-B4F7-E9F43425BC3F}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{86050E56-5CC9-4B13-83E2-66DAEB2AC403}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="14865" yWindow="0" windowWidth="13935" windowHeight="16200" activeTab="2" xr2:uid="{8E82F3E7-134D-474C-9FA7-3A32119CCF80}"/>
+    <workbookView xWindow="-108" yWindow="348" windowWidth="23256" windowHeight="12720" activeTab="2" xr2:uid="{8E82F3E7-134D-474C-9FA7-3A32119CCF80}"/>
   </bookViews>
   <sheets>
     <sheet name="FSM" sheetId="2" r:id="rId1"/>
@@ -41,7 +41,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="268" uniqueCount="92">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="269" uniqueCount="93">
   <si>
     <t>X</t>
   </si>
@@ -318,6 +318,9 @@
   </si>
   <si>
     <t>Prog. Ensamblador</t>
+  </si>
+  <si>
+    <t>#</t>
   </si>
 </sst>
 </file>
@@ -1059,49 +1062,49 @@
     <xf numFmtId="0" fontId="1" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment horizontal="left"/>
     </xf>
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="24" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="13" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="15" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="16" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="2" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="2" borderId="6" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="2" borderId="5" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="21" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="22" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="20" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="2" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
     <xf numFmtId="0" fontId="1" fillId="2" borderId="10" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
     <xf numFmtId="0" fontId="1" fillId="2" borderId="11" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="2" borderId="13" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="2" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="2" borderId="2" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="2" borderId="20" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="2" borderId="24" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="2" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="2" borderId="15" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="2" borderId="16" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="2" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="2" borderId="6" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="2" borderId="5" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="2" borderId="21" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="2" borderId="22" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
@@ -3163,15 +3166,15 @@
       <xdr:twoCellAnchor editAs="oneCell">
         <xdr:from>
           <xdr:col>6</xdr:col>
-          <xdr:colOff>9525</xdr:colOff>
+          <xdr:colOff>7620</xdr:colOff>
           <xdr:row>5</xdr:row>
-          <xdr:rowOff>85725</xdr:rowOff>
+          <xdr:rowOff>83820</xdr:rowOff>
         </xdr:from>
         <xdr:to>
-          <xdr:col>6</xdr:col>
-          <xdr:colOff>1352550</xdr:colOff>
+          <xdr:col>7</xdr:col>
+          <xdr:colOff>30480</xdr:colOff>
           <xdr:row>7</xdr:row>
-          <xdr:rowOff>57150</xdr:rowOff>
+          <xdr:rowOff>45720</xdr:rowOff>
         </xdr:to>
         <xdr:sp macro="" textlink="">
           <xdr:nvSpPr>
@@ -3523,22 +3526,22 @@
       <selection activeCell="N18" sqref="N18"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr baseColWidth="10" defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <cols>
-    <col min="1" max="1" width="3.85546875" style="5" customWidth="1"/>
-    <col min="2" max="2" width="3.85546875" customWidth="1"/>
+    <col min="1" max="1" width="3.88671875" style="5" customWidth="1"/>
+    <col min="2" max="2" width="3.88671875" customWidth="1"/>
     <col min="3" max="3" width="5" customWidth="1"/>
-    <col min="4" max="4" width="6.7109375" customWidth="1"/>
-    <col min="5" max="5" width="6.42578125" customWidth="1"/>
-    <col min="6" max="7" width="4.28515625" style="5" customWidth="1"/>
-    <col min="8" max="8" width="6.85546875" customWidth="1"/>
-    <col min="9" max="12" width="5.28515625" customWidth="1"/>
-    <col min="13" max="15" width="7.28515625" customWidth="1"/>
-    <col min="16" max="41" width="11.42578125" style="5"/>
+    <col min="4" max="4" width="6.6640625" customWidth="1"/>
+    <col min="5" max="5" width="6.44140625" customWidth="1"/>
+    <col min="6" max="7" width="4.33203125" style="5" customWidth="1"/>
+    <col min="8" max="8" width="6.88671875" customWidth="1"/>
+    <col min="9" max="12" width="5.33203125" customWidth="1"/>
+    <col min="13" max="15" width="7.33203125" customWidth="1"/>
+    <col min="16" max="41" width="11.44140625" style="5"/>
   </cols>
   <sheetData>
-    <row r="1" spans="2:15" s="5" customFormat="1" ht="15.75" thickBot="1" x14ac:dyDescent="0.3"/>
-    <row r="2" spans="2:15" s="5" customFormat="1" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="1" spans="2:15" s="5" customFormat="1" ht="15" thickBot="1" x14ac:dyDescent="0.35"/>
+    <row r="2" spans="2:15" s="5" customFormat="1" ht="15" thickBot="1" x14ac:dyDescent="0.35">
       <c r="I2" s="71" t="s">
         <v>7</v>
       </c>
@@ -3548,7 +3551,7 @@
       </c>
       <c r="L2" s="73"/>
     </row>
-    <row r="3" spans="2:15" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="3" spans="2:15" ht="15" thickBot="1" x14ac:dyDescent="0.35">
       <c r="B3" s="74" t="s">
         <v>4</v>
       </c>
@@ -3576,7 +3579,7 @@
         <v>14</v>
       </c>
     </row>
-    <row r="4" spans="2:15" x14ac:dyDescent="0.25">
+    <row r="4" spans="2:15" x14ac:dyDescent="0.3">
       <c r="B4" s="3" t="s">
         <v>2</v>
       </c>
@@ -3614,7 +3617,7 @@
         <v>11</v>
       </c>
     </row>
-    <row r="5" spans="2:15" x14ac:dyDescent="0.25">
+    <row r="5" spans="2:15" x14ac:dyDescent="0.3">
       <c r="B5" s="1">
         <v>0</v>
       </c>
@@ -3652,7 +3655,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="6" spans="2:15" x14ac:dyDescent="0.25">
+    <row r="6" spans="2:15" x14ac:dyDescent="0.3">
       <c r="B6" s="1">
         <v>0</v>
       </c>
@@ -3690,7 +3693,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="7" spans="2:15" x14ac:dyDescent="0.25">
+    <row r="7" spans="2:15" x14ac:dyDescent="0.3">
       <c r="B7" s="1">
         <v>1</v>
       </c>
@@ -3728,7 +3731,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="8" spans="2:15" x14ac:dyDescent="0.25">
+    <row r="8" spans="2:15" x14ac:dyDescent="0.3">
       <c r="B8" s="1">
         <v>1</v>
       </c>
@@ -3766,7 +3769,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="9" spans="2:15" s="5" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="9" spans="2:15" s="5" customFormat="1" x14ac:dyDescent="0.3">
       <c r="H9" s="6">
         <v>1</v>
       </c>
@@ -3792,7 +3795,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="10" spans="2:15" s="5" customFormat="1" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="10" spans="2:15" s="5" customFormat="1" ht="15" thickBot="1" x14ac:dyDescent="0.35">
       <c r="H10" s="6">
         <v>1</v>
       </c>
@@ -3818,7 +3821,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="11" spans="2:15" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="11" spans="2:15" ht="15" thickBot="1" x14ac:dyDescent="0.35">
       <c r="B11" s="74" t="s">
         <v>5</v>
       </c>
@@ -3852,7 +3855,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="12" spans="2:15" x14ac:dyDescent="0.25">
+    <row r="12" spans="2:15" x14ac:dyDescent="0.3">
       <c r="B12" s="3" t="s">
         <v>2</v>
       </c>
@@ -3890,7 +3893,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="13" spans="2:15" x14ac:dyDescent="0.25">
+    <row r="13" spans="2:15" x14ac:dyDescent="0.3">
       <c r="B13" s="1">
         <v>0</v>
       </c>
@@ -3912,7 +3915,7 @@
       <c r="N13" s="5"/>
       <c r="O13" s="5"/>
     </row>
-    <row r="14" spans="2:15" x14ac:dyDescent="0.25">
+    <row r="14" spans="2:15" x14ac:dyDescent="0.3">
       <c r="B14" s="1">
         <v>0</v>
       </c>
@@ -3934,7 +3937,7 @@
       <c r="N14" s="5"/>
       <c r="O14" s="5"/>
     </row>
-    <row r="15" spans="2:15" x14ac:dyDescent="0.25">
+    <row r="15" spans="2:15" x14ac:dyDescent="0.3">
       <c r="B15" s="1">
         <v>1</v>
       </c>
@@ -3956,7 +3959,7 @@
       <c r="N15" s="5"/>
       <c r="O15" s="5"/>
     </row>
-    <row r="16" spans="2:15" x14ac:dyDescent="0.25">
+    <row r="16" spans="2:15" x14ac:dyDescent="0.3">
       <c r="B16" s="1">
         <v>1</v>
       </c>
@@ -3978,12 +3981,12 @@
       <c r="N16" s="5"/>
       <c r="O16" s="5"/>
     </row>
-    <row r="17" s="5" customFormat="1" x14ac:dyDescent="0.25"/>
-    <row r="18" s="5" customFormat="1" x14ac:dyDescent="0.25"/>
-    <row r="19" s="5" customFormat="1" x14ac:dyDescent="0.25"/>
-    <row r="20" s="5" customFormat="1" x14ac:dyDescent="0.25"/>
-    <row r="21" s="5" customFormat="1" x14ac:dyDescent="0.25"/>
-    <row r="22" s="5" customFormat="1" x14ac:dyDescent="0.25"/>
+    <row r="17" s="5" customFormat="1" x14ac:dyDescent="0.3"/>
+    <row r="18" s="5" customFormat="1" x14ac:dyDescent="0.3"/>
+    <row r="19" s="5" customFormat="1" x14ac:dyDescent="0.3"/>
+    <row r="20" s="5" customFormat="1" x14ac:dyDescent="0.3"/>
+    <row r="21" s="5" customFormat="1" x14ac:dyDescent="0.3"/>
+    <row r="22" s="5" customFormat="1" x14ac:dyDescent="0.3"/>
   </sheetData>
   <mergeCells count="8">
     <mergeCell ref="I2:J2"/>
@@ -4009,23 +4012,23 @@
       <selection activeCell="N16" sqref="N16"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr baseColWidth="10" defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <cols>
-    <col min="1" max="1" width="3.85546875" style="5" customWidth="1"/>
-    <col min="2" max="2" width="3.85546875" customWidth="1"/>
+    <col min="1" max="1" width="3.88671875" style="5" customWidth="1"/>
+    <col min="2" max="2" width="3.88671875" customWidth="1"/>
     <col min="3" max="3" width="5" customWidth="1"/>
-    <col min="4" max="4" width="6.7109375" customWidth="1"/>
-    <col min="5" max="5" width="6.42578125" customWidth="1"/>
-    <col min="6" max="7" width="4.28515625" style="5" customWidth="1"/>
-    <col min="8" max="8" width="6.85546875" customWidth="1"/>
-    <col min="9" max="12" width="5.28515625" customWidth="1"/>
-    <col min="13" max="13" width="8.85546875" customWidth="1"/>
-    <col min="14" max="15" width="9.42578125" customWidth="1"/>
-    <col min="16" max="41" width="11.42578125" style="5"/>
+    <col min="4" max="4" width="6.6640625" customWidth="1"/>
+    <col min="5" max="5" width="6.44140625" customWidth="1"/>
+    <col min="6" max="7" width="4.33203125" style="5" customWidth="1"/>
+    <col min="8" max="8" width="6.88671875" customWidth="1"/>
+    <col min="9" max="12" width="5.33203125" customWidth="1"/>
+    <col min="13" max="13" width="8.88671875" customWidth="1"/>
+    <col min="14" max="15" width="9.44140625" customWidth="1"/>
+    <col min="16" max="41" width="11.44140625" style="5"/>
   </cols>
   <sheetData>
-    <row r="1" spans="2:15" s="5" customFormat="1" ht="15.75" thickBot="1" x14ac:dyDescent="0.3"/>
-    <row r="2" spans="2:15" s="5" customFormat="1" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="1" spans="2:15" s="5" customFormat="1" ht="15" thickBot="1" x14ac:dyDescent="0.35"/>
+    <row r="2" spans="2:15" s="5" customFormat="1" ht="15" thickBot="1" x14ac:dyDescent="0.35">
       <c r="I2" s="71" t="s">
         <v>7</v>
       </c>
@@ -4035,7 +4038,7 @@
       </c>
       <c r="L2" s="73"/>
     </row>
-    <row r="3" spans="2:15" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="3" spans="2:15" ht="15" thickBot="1" x14ac:dyDescent="0.35">
       <c r="B3" s="74" t="s">
         <v>4</v>
       </c>
@@ -4063,7 +4066,7 @@
         <v>18</v>
       </c>
     </row>
-    <row r="4" spans="2:15" x14ac:dyDescent="0.25">
+    <row r="4" spans="2:15" x14ac:dyDescent="0.3">
       <c r="B4" s="3" t="s">
         <v>2</v>
       </c>
@@ -4101,7 +4104,7 @@
         <v>20</v>
       </c>
     </row>
-    <row r="5" spans="2:15" x14ac:dyDescent="0.25">
+    <row r="5" spans="2:15" x14ac:dyDescent="0.3">
       <c r="B5" s="1">
         <v>0</v>
       </c>
@@ -4139,7 +4142,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="6" spans="2:15" x14ac:dyDescent="0.25">
+    <row r="6" spans="2:15" x14ac:dyDescent="0.3">
       <c r="B6" s="1">
         <v>0</v>
       </c>
@@ -4177,7 +4180,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="7" spans="2:15" x14ac:dyDescent="0.25">
+    <row r="7" spans="2:15" x14ac:dyDescent="0.3">
       <c r="B7" s="1">
         <v>1</v>
       </c>
@@ -4215,7 +4218,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="8" spans="2:15" x14ac:dyDescent="0.25">
+    <row r="8" spans="2:15" x14ac:dyDescent="0.3">
       <c r="B8" s="1">
         <v>1</v>
       </c>
@@ -4253,7 +4256,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="9" spans="2:15" s="5" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="9" spans="2:15" s="5" customFormat="1" x14ac:dyDescent="0.3">
       <c r="H9" s="6">
         <v>1</v>
       </c>
@@ -4279,7 +4282,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="10" spans="2:15" s="5" customFormat="1" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="10" spans="2:15" s="5" customFormat="1" ht="15" thickBot="1" x14ac:dyDescent="0.35">
       <c r="H10" s="6">
         <v>1</v>
       </c>
@@ -4305,7 +4308,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="11" spans="2:15" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="11" spans="2:15" ht="15" thickBot="1" x14ac:dyDescent="0.35">
       <c r="B11" s="74" t="s">
         <v>5</v>
       </c>
@@ -4339,7 +4342,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="12" spans="2:15" x14ac:dyDescent="0.25">
+    <row r="12" spans="2:15" x14ac:dyDescent="0.3">
       <c r="B12" s="3" t="s">
         <v>2</v>
       </c>
@@ -4377,7 +4380,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="13" spans="2:15" x14ac:dyDescent="0.25">
+    <row r="13" spans="2:15" x14ac:dyDescent="0.3">
       <c r="B13" s="1">
         <v>0</v>
       </c>
@@ -4399,7 +4402,7 @@
       <c r="N13" s="5"/>
       <c r="O13" s="5"/>
     </row>
-    <row r="14" spans="2:15" x14ac:dyDescent="0.25">
+    <row r="14" spans="2:15" x14ac:dyDescent="0.3">
       <c r="B14" s="1">
         <v>0</v>
       </c>
@@ -4423,7 +4426,7 @@
       <c r="N14" s="80"/>
       <c r="O14" s="80"/>
     </row>
-    <row r="15" spans="2:15" x14ac:dyDescent="0.25">
+    <row r="15" spans="2:15" x14ac:dyDescent="0.3">
       <c r="B15" s="1">
         <v>1</v>
       </c>
@@ -4447,7 +4450,7 @@
       <c r="N15" s="80"/>
       <c r="O15" s="80"/>
     </row>
-    <row r="16" spans="2:15" x14ac:dyDescent="0.25">
+    <row r="16" spans="2:15" x14ac:dyDescent="0.3">
       <c r="B16" s="1">
         <v>1</v>
       </c>
@@ -4469,12 +4472,12 @@
       <c r="N16" s="5"/>
       <c r="O16" s="5"/>
     </row>
-    <row r="17" s="5" customFormat="1" x14ac:dyDescent="0.25"/>
-    <row r="18" s="5" customFormat="1" x14ac:dyDescent="0.25"/>
-    <row r="19" s="5" customFormat="1" x14ac:dyDescent="0.25"/>
-    <row r="20" s="5" customFormat="1" x14ac:dyDescent="0.25"/>
-    <row r="21" s="5" customFormat="1" x14ac:dyDescent="0.25"/>
-    <row r="22" s="5" customFormat="1" x14ac:dyDescent="0.25"/>
+    <row r="17" s="5" customFormat="1" x14ac:dyDescent="0.3"/>
+    <row r="18" s="5" customFormat="1" x14ac:dyDescent="0.3"/>
+    <row r="19" s="5" customFormat="1" x14ac:dyDescent="0.3"/>
+    <row r="20" s="5" customFormat="1" x14ac:dyDescent="0.3"/>
+    <row r="21" s="5" customFormat="1" x14ac:dyDescent="0.3"/>
+    <row r="22" s="5" customFormat="1" x14ac:dyDescent="0.3"/>
   </sheetData>
   <mergeCells count="10">
     <mergeCell ref="B11:C11"/>
@@ -4498,27 +4501,27 @@
   <sheetPr codeName="Hoja3"/>
   <dimension ref="A1:AP187"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A17" zoomScale="120" zoomScaleNormal="120" workbookViewId="0">
-      <selection activeCell="I35" sqref="I35"/>
+    <sheetView tabSelected="1" topLeftCell="A25" zoomScale="120" zoomScaleNormal="120" workbookViewId="0">
+      <selection activeCell="A29" sqref="A29"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr baseColWidth="10" defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <cols>
-    <col min="1" max="1" width="3.85546875" style="5" customWidth="1"/>
-    <col min="2" max="2" width="3.85546875" customWidth="1"/>
+    <col min="1" max="1" width="3.88671875" style="5" customWidth="1"/>
+    <col min="2" max="2" width="3.88671875" customWidth="1"/>
     <col min="3" max="3" width="5" customWidth="1"/>
-    <col min="4" max="4" width="6.7109375" customWidth="1"/>
-    <col min="5" max="5" width="6.42578125" customWidth="1"/>
-    <col min="6" max="7" width="4.28515625" style="5" customWidth="1"/>
-    <col min="8" max="8" width="6.85546875" customWidth="1"/>
-    <col min="9" max="12" width="5.28515625" customWidth="1"/>
-    <col min="13" max="13" width="8.85546875" customWidth="1"/>
-    <col min="14" max="16" width="9.42578125" customWidth="1"/>
-    <col min="17" max="42" width="11.42578125" style="5"/>
+    <col min="4" max="4" width="6.6640625" customWidth="1"/>
+    <col min="5" max="5" width="6.44140625" customWidth="1"/>
+    <col min="6" max="7" width="4.33203125" style="5" customWidth="1"/>
+    <col min="8" max="8" width="6.88671875" customWidth="1"/>
+    <col min="9" max="12" width="5.33203125" customWidth="1"/>
+    <col min="13" max="13" width="8.88671875" customWidth="1"/>
+    <col min="14" max="16" width="9.44140625" customWidth="1"/>
+    <col min="17" max="42" width="11.44140625" style="5"/>
   </cols>
   <sheetData>
-    <row r="1" spans="2:16" s="5" customFormat="1" ht="15.75" thickBot="1" x14ac:dyDescent="0.3"/>
-    <row r="2" spans="2:16" s="5" customFormat="1" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="1" spans="2:16" s="5" customFormat="1" ht="15" thickBot="1" x14ac:dyDescent="0.35"/>
+    <row r="2" spans="2:16" s="5" customFormat="1" ht="15" thickBot="1" x14ac:dyDescent="0.35">
       <c r="I2" s="71" t="s">
         <v>7</v>
       </c>
@@ -4528,7 +4531,7 @@
       </c>
       <c r="L2" s="73"/>
     </row>
-    <row r="3" spans="2:16" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="3" spans="2:16" ht="15" thickBot="1" x14ac:dyDescent="0.35">
       <c r="B3" s="74" t="s">
         <v>4</v>
       </c>
@@ -4559,7 +4562,7 @@
         <v>18</v>
       </c>
     </row>
-    <row r="4" spans="2:16" x14ac:dyDescent="0.25">
+    <row r="4" spans="2:16" x14ac:dyDescent="0.3">
       <c r="B4" s="3" t="s">
         <v>2</v>
       </c>
@@ -4600,7 +4603,7 @@
         <v>20</v>
       </c>
     </row>
-    <row r="5" spans="2:16" x14ac:dyDescent="0.25">
+    <row r="5" spans="2:16" x14ac:dyDescent="0.3">
       <c r="B5" s="1">
         <v>0</v>
       </c>
@@ -4641,7 +4644,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="6" spans="2:16" x14ac:dyDescent="0.25">
+    <row r="6" spans="2:16" x14ac:dyDescent="0.3">
       <c r="B6" s="1">
         <v>0</v>
       </c>
@@ -4682,7 +4685,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="7" spans="2:16" x14ac:dyDescent="0.25">
+    <row r="7" spans="2:16" x14ac:dyDescent="0.3">
       <c r="B7" s="1">
         <v>1</v>
       </c>
@@ -4723,7 +4726,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="8" spans="2:16" x14ac:dyDescent="0.25">
+    <row r="8" spans="2:16" x14ac:dyDescent="0.3">
       <c r="B8" s="1">
         <v>1</v>
       </c>
@@ -4764,7 +4767,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="9" spans="2:16" s="5" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="9" spans="2:16" s="5" customFormat="1" x14ac:dyDescent="0.3">
       <c r="H9" s="19">
         <v>1</v>
       </c>
@@ -4793,7 +4796,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="10" spans="2:16" s="5" customFormat="1" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="10" spans="2:16" s="5" customFormat="1" ht="15" thickBot="1" x14ac:dyDescent="0.35">
       <c r="H10" s="19">
         <v>1</v>
       </c>
@@ -4822,7 +4825,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="11" spans="2:16" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="11" spans="2:16" ht="15" thickBot="1" x14ac:dyDescent="0.35">
       <c r="B11" s="74" t="s">
         <v>5</v>
       </c>
@@ -4859,7 +4862,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="12" spans="2:16" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="12" spans="2:16" ht="15" thickBot="1" x14ac:dyDescent="0.35">
       <c r="B12" s="3" t="s">
         <v>2</v>
       </c>
@@ -4900,7 +4903,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="13" spans="2:16" x14ac:dyDescent="0.25">
+    <row r="13" spans="2:16" x14ac:dyDescent="0.3">
       <c r="B13" s="1">
         <v>0</v>
       </c>
@@ -4923,7 +4926,7 @@
       <c r="O13" s="5"/>
       <c r="P13" s="5"/>
     </row>
-    <row r="14" spans="2:16" x14ac:dyDescent="0.25">
+    <row r="14" spans="2:16" x14ac:dyDescent="0.3">
       <c r="B14" s="1">
         <v>0</v>
       </c>
@@ -4952,7 +4955,7 @@
       </c>
       <c r="P14" s="80"/>
     </row>
-    <row r="15" spans="2:16" x14ac:dyDescent="0.25">
+    <row r="15" spans="2:16" x14ac:dyDescent="0.3">
       <c r="B15" s="1">
         <v>1</v>
       </c>
@@ -4981,7 +4984,7 @@
       </c>
       <c r="P15" s="80"/>
     </row>
-    <row r="16" spans="2:16" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="16" spans="2:16" ht="15" thickBot="1" x14ac:dyDescent="0.35">
       <c r="B16" s="1">
         <v>1</v>
       </c>
@@ -5004,21 +5007,21 @@
       <c r="O16" s="5"/>
       <c r="P16" s="5"/>
     </row>
-    <row r="17" spans="2:16" s="5" customFormat="1" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="H17" s="91" t="s">
+    <row r="17" spans="1:16" s="5" customFormat="1" ht="15" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="H17" s="87" t="s">
         <v>23</v>
       </c>
-      <c r="I17" s="93"/>
-      <c r="J17" s="93"/>
-      <c r="K17" s="93"/>
-      <c r="L17" s="92"/>
-      <c r="M17" s="91" t="s">
+      <c r="I17" s="89"/>
+      <c r="J17" s="89"/>
+      <c r="K17" s="89"/>
+      <c r="L17" s="88"/>
+      <c r="M17" s="87" t="s">
         <v>44</v>
       </c>
-      <c r="N17" s="92"/>
+      <c r="N17" s="88"/>
       <c r="O17" s="29"/>
     </row>
-    <row r="18" spans="2:16" s="5" customFormat="1" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="18" spans="1:16" s="5" customFormat="1" ht="15" thickBot="1" x14ac:dyDescent="0.35">
       <c r="B18" s="74" t="s">
         <v>52</v>
       </c>
@@ -5027,15 +5030,15 @@
         <v>6</v>
       </c>
       <c r="E18" s="77"/>
-      <c r="H18" s="81" t="s">
+      <c r="H18" s="94" t="s">
         <v>24</v>
       </c>
-      <c r="I18" s="82"/>
-      <c r="J18" s="82"/>
-      <c r="K18" s="82" t="s">
+      <c r="I18" s="95"/>
+      <c r="J18" s="95"/>
+      <c r="K18" s="95" t="s">
         <v>35</v>
       </c>
-      <c r="L18" s="82"/>
+      <c r="L18" s="95"/>
       <c r="M18" s="10" t="s">
         <v>25</v>
       </c>
@@ -5044,7 +5047,7 @@
       </c>
       <c r="O18" s="30"/>
     </row>
-    <row r="19" spans="2:16" s="5" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="19" spans="1:16" s="5" customFormat="1" x14ac:dyDescent="0.3">
       <c r="B19" s="3" t="s">
         <v>2</v>
       </c>
@@ -5057,15 +5060,15 @@
       <c r="E19" s="3" t="s">
         <v>0</v>
       </c>
-      <c r="H19" s="83" t="s">
+      <c r="H19" s="84" t="s">
         <v>30</v>
       </c>
-      <c r="I19" s="84"/>
-      <c r="J19" s="84"/>
-      <c r="K19" s="84" t="s">
+      <c r="I19" s="81"/>
+      <c r="J19" s="81"/>
+      <c r="K19" s="81" t="s">
         <v>31</v>
       </c>
-      <c r="L19" s="84"/>
+      <c r="L19" s="81"/>
       <c r="M19" s="11" t="s">
         <v>39</v>
       </c>
@@ -5074,7 +5077,7 @@
       </c>
       <c r="O19" s="31"/>
     </row>
-    <row r="20" spans="2:16" s="5" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="20" spans="1:16" s="5" customFormat="1" x14ac:dyDescent="0.3">
       <c r="B20" s="1">
         <v>0</v>
       </c>
@@ -5087,15 +5090,15 @@
       <c r="E20" s="2">
         <v>1</v>
       </c>
-      <c r="H20" s="83" t="s">
+      <c r="H20" s="84" t="s">
         <v>32</v>
       </c>
-      <c r="I20" s="84"/>
-      <c r="J20" s="84"/>
-      <c r="K20" s="84" t="s">
+      <c r="I20" s="81"/>
+      <c r="J20" s="81"/>
+      <c r="K20" s="81" t="s">
         <v>33</v>
       </c>
-      <c r="L20" s="84"/>
+      <c r="L20" s="81"/>
       <c r="M20" s="11" t="s">
         <v>37</v>
       </c>
@@ -5104,7 +5107,7 @@
       </c>
       <c r="O20" s="32"/>
     </row>
-    <row r="21" spans="2:16" s="5" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="21" spans="1:16" s="5" customFormat="1" x14ac:dyDescent="0.3">
       <c r="B21" s="1">
         <v>0</v>
       </c>
@@ -5113,15 +5116,15 @@
       </c>
       <c r="D21" s="2"/>
       <c r="E21" s="2"/>
-      <c r="H21" s="83" t="s">
+      <c r="H21" s="84" t="s">
         <v>43</v>
       </c>
-      <c r="I21" s="84"/>
-      <c r="J21" s="84"/>
-      <c r="K21" s="84" t="s">
+      <c r="I21" s="81"/>
+      <c r="J21" s="81"/>
+      <c r="K21" s="81" t="s">
         <v>36</v>
       </c>
-      <c r="L21" s="84"/>
+      <c r="L21" s="81"/>
       <c r="M21" s="11" t="s">
         <v>38</v>
       </c>
@@ -5130,7 +5133,7 @@
       </c>
       <c r="O21" s="32"/>
     </row>
-    <row r="22" spans="2:16" s="5" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="22" spans="1:16" s="5" customFormat="1" x14ac:dyDescent="0.3">
       <c r="B22" s="1">
         <v>1</v>
       </c>
@@ -5139,15 +5142,15 @@
       </c>
       <c r="D22" s="2"/>
       <c r="E22" s="2"/>
-      <c r="H22" s="94" t="s">
+      <c r="H22" s="90" t="s">
         <v>27</v>
       </c>
-      <c r="I22" s="95"/>
-      <c r="J22" s="86"/>
-      <c r="K22" s="85" t="s">
+      <c r="I22" s="91"/>
+      <c r="J22" s="92"/>
+      <c r="K22" s="93" t="s">
         <v>29</v>
       </c>
-      <c r="L22" s="86"/>
+      <c r="L22" s="92"/>
       <c r="M22" s="11" t="s">
         <v>40</v>
       </c>
@@ -5156,7 +5159,7 @@
       </c>
       <c r="O22" s="31"/>
     </row>
-    <row r="23" spans="2:16" s="5" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="23" spans="1:16" s="5" customFormat="1" x14ac:dyDescent="0.3">
       <c r="B23" s="1">
         <v>1</v>
       </c>
@@ -5165,15 +5168,15 @@
       </c>
       <c r="D23" s="2"/>
       <c r="E23" s="2"/>
-      <c r="H23" s="83" t="s">
+      <c r="H23" s="84" t="s">
         <v>28</v>
       </c>
-      <c r="I23" s="84"/>
-      <c r="J23" s="84"/>
-      <c r="K23" s="84" t="s">
+      <c r="I23" s="81"/>
+      <c r="J23" s="81"/>
+      <c r="K23" s="81" t="s">
         <v>26</v>
       </c>
-      <c r="L23" s="84"/>
+      <c r="L23" s="81"/>
       <c r="M23" s="11" t="s">
         <v>41</v>
       </c>
@@ -5182,36 +5185,36 @@
       </c>
       <c r="O23" s="32"/>
     </row>
-    <row r="24" spans="2:16" s="5" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="H24" s="83"/>
-      <c r="I24" s="84"/>
-      <c r="J24" s="84"/>
-      <c r="K24" s="84"/>
-      <c r="L24" s="84"/>
+    <row r="24" spans="1:16" s="5" customFormat="1" x14ac:dyDescent="0.3">
+      <c r="H24" s="84"/>
+      <c r="I24" s="81"/>
+      <c r="J24" s="81"/>
+      <c r="K24" s="81"/>
+      <c r="L24" s="81"/>
       <c r="M24" s="9"/>
       <c r="N24" s="12"/>
       <c r="O24" s="32"/>
     </row>
-    <row r="25" spans="2:16" s="5" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="H25" s="83"/>
-      <c r="I25" s="84"/>
-      <c r="J25" s="84"/>
-      <c r="K25" s="84"/>
-      <c r="L25" s="84"/>
+    <row r="25" spans="1:16" s="5" customFormat="1" x14ac:dyDescent="0.3">
+      <c r="H25" s="84"/>
+      <c r="I25" s="81"/>
+      <c r="J25" s="81"/>
+      <c r="K25" s="81"/>
+      <c r="L25" s="81"/>
       <c r="M25" s="9"/>
       <c r="N25" s="12"/>
       <c r="O25" s="32"/>
     </row>
-    <row r="26" spans="2:16" s="5" customFormat="1" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="H26" s="89" t="s">
+    <row r="26" spans="1:16" s="5" customFormat="1" ht="15" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="H26" s="85" t="s">
         <v>45</v>
       </c>
-      <c r="I26" s="90"/>
-      <c r="J26" s="90"/>
-      <c r="K26" s="90" t="s">
+      <c r="I26" s="86"/>
+      <c r="J26" s="86"/>
+      <c r="K26" s="86" t="s">
         <v>46</v>
       </c>
-      <c r="L26" s="90"/>
+      <c r="L26" s="86"/>
       <c r="M26" s="15" t="s">
         <v>47</v>
       </c>
@@ -5220,31 +5223,34 @@
       </c>
       <c r="O26" s="31"/>
     </row>
-    <row r="27" spans="2:16" s="5" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="B27" s="84" t="s">
+    <row r="27" spans="1:16" s="5" customFormat="1" x14ac:dyDescent="0.3">
+      <c r="B27" s="81" t="s">
         <v>68</v>
       </c>
-      <c r="C27" s="84"/>
-      <c r="D27" s="84"/>
-      <c r="E27" s="84"/>
-      <c r="F27" s="84"/>
-      <c r="G27" s="84"/>
-    </row>
-    <row r="28" spans="2:16" s="5" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="C27" s="81"/>
+      <c r="D27" s="81"/>
+      <c r="E27" s="81"/>
+      <c r="F27" s="81"/>
+      <c r="G27" s="81"/>
+    </row>
+    <row r="28" spans="1:16" s="5" customFormat="1" x14ac:dyDescent="0.3">
       <c r="B28" s="33" t="s">
         <v>69</v>
       </c>
-      <c r="C28" s="84" t="s">
+      <c r="C28" s="81" t="s">
         <v>70</v>
       </c>
-      <c r="D28" s="84"/>
-      <c r="E28" s="84"/>
-      <c r="F28" s="84" t="s">
+      <c r="D28" s="81"/>
+      <c r="E28" s="81"/>
+      <c r="F28" s="81" t="s">
         <v>18</v>
       </c>
-      <c r="G28" s="84"/>
-    </row>
-    <row r="29" spans="2:16" s="5" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="G28" s="81"/>
+    </row>
+    <row r="29" spans="1:16" s="5" customFormat="1" x14ac:dyDescent="0.3">
+      <c r="A29" s="32" t="s">
+        <v>92</v>
+      </c>
       <c r="B29" s="69" t="s">
         <v>61</v>
       </c>
@@ -5268,7 +5274,10 @@
       <c r="O29" s="6"/>
       <c r="P29" s="6"/>
     </row>
-    <row r="30" spans="2:16" s="5" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="30" spans="1:16" s="5" customFormat="1" x14ac:dyDescent="0.3">
+      <c r="A30" s="32">
+        <v>0</v>
+      </c>
       <c r="B30" s="33">
         <v>0</v>
       </c>
@@ -5288,7 +5297,10 @@
         <v>0</v>
       </c>
     </row>
-    <row r="31" spans="2:16" s="5" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="31" spans="1:16" s="5" customFormat="1" x14ac:dyDescent="0.3">
+      <c r="A31" s="32">
+        <v>1</v>
+      </c>
       <c r="B31" s="33">
         <v>0</v>
       </c>
@@ -5323,7 +5335,10 @@
         <v>76</v>
       </c>
     </row>
-    <row r="32" spans="2:16" s="5" customFormat="1" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="32" spans="1:16" s="5" customFormat="1" ht="15" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="A32" s="32">
+        <v>2</v>
+      </c>
       <c r="B32" s="33">
         <v>0</v>
       </c>
@@ -5361,7 +5376,10 @@
         <v>75</v>
       </c>
     </row>
-    <row r="33" spans="2:16" s="5" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="33" spans="1:16" s="5" customFormat="1" x14ac:dyDescent="0.3">
+      <c r="A33" s="32">
+        <v>3</v>
+      </c>
       <c r="B33" s="33">
         <v>0</v>
       </c>
@@ -5391,7 +5409,10 @@
       <c r="O33" s="37"/>
       <c r="P33" s="41"/>
     </row>
-    <row r="34" spans="2:16" s="5" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="34" spans="1:16" s="5" customFormat="1" x14ac:dyDescent="0.3">
+      <c r="A34" s="32">
+        <v>4</v>
+      </c>
       <c r="B34" s="33">
         <v>0</v>
       </c>
@@ -5421,7 +5442,10 @@
       <c r="O34" s="6"/>
       <c r="P34" s="12"/>
     </row>
-    <row r="35" spans="2:16" s="5" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="35" spans="1:16" s="5" customFormat="1" x14ac:dyDescent="0.3">
+      <c r="A35" s="32">
+        <v>5</v>
+      </c>
       <c r="B35" s="33">
         <v>0</v>
       </c>
@@ -5459,7 +5483,10 @@
         <v>1</v>
       </c>
     </row>
-    <row r="36" spans="2:16" s="5" customFormat="1" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="36" spans="1:16" s="5" customFormat="1" ht="15" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="A36" s="32">
+        <v>6</v>
+      </c>
       <c r="B36" s="33">
         <v>0</v>
       </c>
@@ -5491,7 +5518,10 @@
         <v>1</v>
       </c>
     </row>
-    <row r="37" spans="2:16" s="5" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="37" spans="1:16" s="5" customFormat="1" x14ac:dyDescent="0.3">
+      <c r="A37" s="32">
+        <v>7</v>
+      </c>
       <c r="B37" s="33">
         <v>0</v>
       </c>
@@ -5510,14 +5540,17 @@
       <c r="G37" s="33">
         <v>0</v>
       </c>
-      <c r="M37" s="87" t="s">
+      <c r="M37" s="82" t="s">
         <v>77</v>
       </c>
-      <c r="N37" s="87"/>
-      <c r="O37" s="87"/>
-      <c r="P37" s="87"/>
-    </row>
-    <row r="38" spans="2:16" s="5" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="N37" s="82"/>
+      <c r="O37" s="82"/>
+      <c r="P37" s="82"/>
+    </row>
+    <row r="38" spans="1:16" s="5" customFormat="1" x14ac:dyDescent="0.3">
+      <c r="A38" s="32">
+        <v>8</v>
+      </c>
       <c r="B38" s="33">
         <v>1</v>
       </c>
@@ -5537,7 +5570,10 @@
         <v>0</v>
       </c>
     </row>
-    <row r="39" spans="2:16" s="5" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="39" spans="1:16" s="5" customFormat="1" x14ac:dyDescent="0.3">
+      <c r="A39" s="32">
+        <v>9</v>
+      </c>
       <c r="B39" s="33">
         <v>1</v>
       </c>
@@ -5572,7 +5608,10 @@
         <v>76</v>
       </c>
     </row>
-    <row r="40" spans="2:16" s="5" customFormat="1" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="40" spans="1:16" s="5" customFormat="1" ht="15" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="A40" s="32">
+        <v>10</v>
+      </c>
       <c r="B40" s="33">
         <v>1</v>
       </c>
@@ -5610,7 +5649,10 @@
         <v>75</v>
       </c>
     </row>
-    <row r="41" spans="2:16" s="5" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="41" spans="1:16" s="5" customFormat="1" x14ac:dyDescent="0.3">
+      <c r="A41" s="32">
+        <v>11</v>
+      </c>
       <c r="B41" s="33">
         <v>1</v>
       </c>
@@ -5640,7 +5682,10 @@
       <c r="O41" s="37"/>
       <c r="P41" s="41"/>
     </row>
-    <row r="42" spans="2:16" s="5" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="42" spans="1:16" s="5" customFormat="1" x14ac:dyDescent="0.3">
+      <c r="A42" s="32">
+        <v>12</v>
+      </c>
       <c r="B42" s="33">
         <v>1</v>
       </c>
@@ -5670,7 +5715,10 @@
       <c r="O42" s="6"/>
       <c r="P42" s="12"/>
     </row>
-    <row r="43" spans="2:16" s="5" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="43" spans="1:16" s="5" customFormat="1" x14ac:dyDescent="0.3">
+      <c r="A43" s="32">
+        <v>13</v>
+      </c>
       <c r="B43" s="33">
         <v>1</v>
       </c>
@@ -5708,7 +5756,10 @@
         <v>1</v>
       </c>
     </row>
-    <row r="44" spans="2:16" s="5" customFormat="1" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="44" spans="1:16" s="5" customFormat="1" ht="15" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="A44" s="32">
+        <v>14</v>
+      </c>
       <c r="B44" s="33">
         <v>1</v>
       </c>
@@ -5740,7 +5791,10 @@
       <c r="O44" s="43"/>
       <c r="P44" s="44"/>
     </row>
-    <row r="45" spans="2:16" s="5" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="45" spans="1:16" s="5" customFormat="1" x14ac:dyDescent="0.3">
+      <c r="A45" s="32">
+        <v>15</v>
+      </c>
       <c r="B45" s="33">
         <v>1</v>
       </c>
@@ -5759,159 +5813,184 @@
       <c r="G45" s="39">
         <v>1</v>
       </c>
-      <c r="K45" s="88" t="s">
+      <c r="K45" s="83" t="s">
         <v>78</v>
       </c>
-      <c r="L45" s="88"/>
-      <c r="M45" s="88"/>
-      <c r="N45" s="88"/>
-      <c r="O45" s="88"/>
-      <c r="P45" s="88"/>
-    </row>
-    <row r="46" spans="2:16" s="5" customFormat="1" x14ac:dyDescent="0.25"/>
-    <row r="47" spans="2:16" s="5" customFormat="1" x14ac:dyDescent="0.25"/>
-    <row r="48" spans="2:16" s="5" customFormat="1" x14ac:dyDescent="0.25"/>
-    <row r="49" s="5" customFormat="1" x14ac:dyDescent="0.25"/>
-    <row r="50" s="5" customFormat="1" x14ac:dyDescent="0.25"/>
-    <row r="51" s="5" customFormat="1" x14ac:dyDescent="0.25"/>
-    <row r="52" s="5" customFormat="1" x14ac:dyDescent="0.25"/>
-    <row r="53" s="5" customFormat="1" x14ac:dyDescent="0.25"/>
-    <row r="54" s="5" customFormat="1" x14ac:dyDescent="0.25"/>
-    <row r="55" s="5" customFormat="1" x14ac:dyDescent="0.25"/>
-    <row r="56" s="5" customFormat="1" x14ac:dyDescent="0.25"/>
-    <row r="57" s="5" customFormat="1" x14ac:dyDescent="0.25"/>
-    <row r="58" s="5" customFormat="1" x14ac:dyDescent="0.25"/>
-    <row r="59" s="5" customFormat="1" x14ac:dyDescent="0.25"/>
-    <row r="60" s="5" customFormat="1" x14ac:dyDescent="0.25"/>
-    <row r="61" s="5" customFormat="1" x14ac:dyDescent="0.25"/>
-    <row r="62" s="5" customFormat="1" x14ac:dyDescent="0.25"/>
-    <row r="63" s="5" customFormat="1" x14ac:dyDescent="0.25"/>
-    <row r="64" s="5" customFormat="1" x14ac:dyDescent="0.25"/>
-    <row r="65" s="5" customFormat="1" x14ac:dyDescent="0.25"/>
-    <row r="66" s="5" customFormat="1" x14ac:dyDescent="0.25"/>
-    <row r="67" s="5" customFormat="1" x14ac:dyDescent="0.25"/>
-    <row r="68" s="5" customFormat="1" x14ac:dyDescent="0.25"/>
-    <row r="69" s="5" customFormat="1" x14ac:dyDescent="0.25"/>
-    <row r="70" s="5" customFormat="1" x14ac:dyDescent="0.25"/>
-    <row r="71" s="5" customFormat="1" x14ac:dyDescent="0.25"/>
-    <row r="72" s="5" customFormat="1" x14ac:dyDescent="0.25"/>
-    <row r="73" s="5" customFormat="1" x14ac:dyDescent="0.25"/>
-    <row r="74" s="5" customFormat="1" x14ac:dyDescent="0.25"/>
-    <row r="75" s="5" customFormat="1" x14ac:dyDescent="0.25"/>
-    <row r="76" s="5" customFormat="1" x14ac:dyDescent="0.25"/>
-    <row r="77" s="5" customFormat="1" x14ac:dyDescent="0.25"/>
-    <row r="78" s="5" customFormat="1" x14ac:dyDescent="0.25"/>
-    <row r="79" s="5" customFormat="1" x14ac:dyDescent="0.25"/>
-    <row r="80" s="5" customFormat="1" x14ac:dyDescent="0.25"/>
-    <row r="81" s="5" customFormat="1" x14ac:dyDescent="0.25"/>
-    <row r="82" s="5" customFormat="1" x14ac:dyDescent="0.25"/>
-    <row r="83" s="5" customFormat="1" x14ac:dyDescent="0.25"/>
-    <row r="84" s="5" customFormat="1" x14ac:dyDescent="0.25"/>
-    <row r="85" s="5" customFormat="1" x14ac:dyDescent="0.25"/>
-    <row r="86" s="5" customFormat="1" x14ac:dyDescent="0.25"/>
-    <row r="87" s="5" customFormat="1" x14ac:dyDescent="0.25"/>
-    <row r="88" s="5" customFormat="1" x14ac:dyDescent="0.25"/>
-    <row r="89" s="5" customFormat="1" x14ac:dyDescent="0.25"/>
-    <row r="90" s="5" customFormat="1" x14ac:dyDescent="0.25"/>
-    <row r="91" s="5" customFormat="1" x14ac:dyDescent="0.25"/>
-    <row r="92" s="5" customFormat="1" x14ac:dyDescent="0.25"/>
-    <row r="93" s="5" customFormat="1" x14ac:dyDescent="0.25"/>
-    <row r="94" s="5" customFormat="1" x14ac:dyDescent="0.25"/>
-    <row r="95" s="5" customFormat="1" x14ac:dyDescent="0.25"/>
-    <row r="96" s="5" customFormat="1" x14ac:dyDescent="0.25"/>
-    <row r="97" s="5" customFormat="1" x14ac:dyDescent="0.25"/>
-    <row r="98" s="5" customFormat="1" x14ac:dyDescent="0.25"/>
-    <row r="99" s="5" customFormat="1" x14ac:dyDescent="0.25"/>
-    <row r="100" s="5" customFormat="1" x14ac:dyDescent="0.25"/>
-    <row r="101" s="5" customFormat="1" x14ac:dyDescent="0.25"/>
-    <row r="102" s="5" customFormat="1" x14ac:dyDescent="0.25"/>
-    <row r="103" s="5" customFormat="1" x14ac:dyDescent="0.25"/>
-    <row r="104" s="5" customFormat="1" x14ac:dyDescent="0.25"/>
-    <row r="105" s="5" customFormat="1" x14ac:dyDescent="0.25"/>
-    <row r="106" s="5" customFormat="1" x14ac:dyDescent="0.25"/>
-    <row r="107" s="5" customFormat="1" x14ac:dyDescent="0.25"/>
-    <row r="108" s="5" customFormat="1" x14ac:dyDescent="0.25"/>
-    <row r="109" s="5" customFormat="1" x14ac:dyDescent="0.25"/>
-    <row r="110" s="5" customFormat="1" x14ac:dyDescent="0.25"/>
-    <row r="111" s="5" customFormat="1" x14ac:dyDescent="0.25"/>
-    <row r="112" s="5" customFormat="1" x14ac:dyDescent="0.25"/>
-    <row r="113" s="5" customFormat="1" x14ac:dyDescent="0.25"/>
-    <row r="114" s="5" customFormat="1" x14ac:dyDescent="0.25"/>
-    <row r="115" s="5" customFormat="1" x14ac:dyDescent="0.25"/>
-    <row r="116" s="5" customFormat="1" x14ac:dyDescent="0.25"/>
-    <row r="117" s="5" customFormat="1" x14ac:dyDescent="0.25"/>
-    <row r="118" s="5" customFormat="1" x14ac:dyDescent="0.25"/>
-    <row r="119" s="5" customFormat="1" x14ac:dyDescent="0.25"/>
-    <row r="120" s="5" customFormat="1" x14ac:dyDescent="0.25"/>
-    <row r="121" s="5" customFormat="1" x14ac:dyDescent="0.25"/>
-    <row r="122" s="5" customFormat="1" x14ac:dyDescent="0.25"/>
-    <row r="123" s="5" customFormat="1" x14ac:dyDescent="0.25"/>
-    <row r="124" s="5" customFormat="1" x14ac:dyDescent="0.25"/>
-    <row r="125" s="5" customFormat="1" x14ac:dyDescent="0.25"/>
-    <row r="126" s="5" customFormat="1" x14ac:dyDescent="0.25"/>
-    <row r="127" s="5" customFormat="1" x14ac:dyDescent="0.25"/>
-    <row r="128" s="5" customFormat="1" x14ac:dyDescent="0.25"/>
-    <row r="129" s="5" customFormat="1" x14ac:dyDescent="0.25"/>
-    <row r="130" s="5" customFormat="1" x14ac:dyDescent="0.25"/>
-    <row r="131" s="5" customFormat="1" x14ac:dyDescent="0.25"/>
-    <row r="132" s="5" customFormat="1" x14ac:dyDescent="0.25"/>
-    <row r="133" s="5" customFormat="1" x14ac:dyDescent="0.25"/>
-    <row r="134" s="5" customFormat="1" x14ac:dyDescent="0.25"/>
-    <row r="135" s="5" customFormat="1" x14ac:dyDescent="0.25"/>
-    <row r="136" s="5" customFormat="1" x14ac:dyDescent="0.25"/>
-    <row r="137" s="5" customFormat="1" x14ac:dyDescent="0.25"/>
-    <row r="138" s="5" customFormat="1" x14ac:dyDescent="0.25"/>
-    <row r="139" s="5" customFormat="1" x14ac:dyDescent="0.25"/>
-    <row r="140" s="5" customFormat="1" x14ac:dyDescent="0.25"/>
-    <row r="141" s="5" customFormat="1" x14ac:dyDescent="0.25"/>
-    <row r="142" s="5" customFormat="1" x14ac:dyDescent="0.25"/>
-    <row r="143" s="5" customFormat="1" x14ac:dyDescent="0.25"/>
-    <row r="144" s="5" customFormat="1" x14ac:dyDescent="0.25"/>
-    <row r="145" s="5" customFormat="1" x14ac:dyDescent="0.25"/>
-    <row r="146" s="5" customFormat="1" x14ac:dyDescent="0.25"/>
-    <row r="147" s="5" customFormat="1" x14ac:dyDescent="0.25"/>
-    <row r="148" s="5" customFormat="1" x14ac:dyDescent="0.25"/>
-    <row r="149" s="5" customFormat="1" x14ac:dyDescent="0.25"/>
-    <row r="150" s="5" customFormat="1" x14ac:dyDescent="0.25"/>
-    <row r="151" s="5" customFormat="1" x14ac:dyDescent="0.25"/>
-    <row r="152" s="5" customFormat="1" x14ac:dyDescent="0.25"/>
-    <row r="153" s="5" customFormat="1" x14ac:dyDescent="0.25"/>
-    <row r="154" s="5" customFormat="1" x14ac:dyDescent="0.25"/>
-    <row r="155" s="5" customFormat="1" x14ac:dyDescent="0.25"/>
-    <row r="156" s="5" customFormat="1" x14ac:dyDescent="0.25"/>
-    <row r="157" s="5" customFormat="1" x14ac:dyDescent="0.25"/>
-    <row r="158" s="5" customFormat="1" x14ac:dyDescent="0.25"/>
-    <row r="159" s="5" customFormat="1" x14ac:dyDescent="0.25"/>
-    <row r="160" s="5" customFormat="1" x14ac:dyDescent="0.25"/>
-    <row r="161" s="5" customFormat="1" x14ac:dyDescent="0.25"/>
-    <row r="162" s="5" customFormat="1" x14ac:dyDescent="0.25"/>
-    <row r="163" s="5" customFormat="1" x14ac:dyDescent="0.25"/>
-    <row r="164" s="5" customFormat="1" x14ac:dyDescent="0.25"/>
-    <row r="165" s="5" customFormat="1" x14ac:dyDescent="0.25"/>
-    <row r="166" s="5" customFormat="1" x14ac:dyDescent="0.25"/>
-    <row r="167" s="5" customFormat="1" x14ac:dyDescent="0.25"/>
-    <row r="168" s="5" customFormat="1" x14ac:dyDescent="0.25"/>
-    <row r="169" s="5" customFormat="1" x14ac:dyDescent="0.25"/>
-    <row r="170" s="5" customFormat="1" x14ac:dyDescent="0.25"/>
-    <row r="171" s="5" customFormat="1" x14ac:dyDescent="0.25"/>
-    <row r="172" s="5" customFormat="1" x14ac:dyDescent="0.25"/>
-    <row r="173" s="5" customFormat="1" x14ac:dyDescent="0.25"/>
-    <row r="174" s="5" customFormat="1" x14ac:dyDescent="0.25"/>
-    <row r="175" s="5" customFormat="1" x14ac:dyDescent="0.25"/>
-    <row r="176" s="5" customFormat="1" x14ac:dyDescent="0.25"/>
-    <row r="177" s="5" customFormat="1" x14ac:dyDescent="0.25"/>
-    <row r="178" s="5" customFormat="1" x14ac:dyDescent="0.25"/>
-    <row r="179" s="5" customFormat="1" x14ac:dyDescent="0.25"/>
-    <row r="180" s="5" customFormat="1" x14ac:dyDescent="0.25"/>
-    <row r="181" s="5" customFormat="1" x14ac:dyDescent="0.25"/>
-    <row r="182" s="5" customFormat="1" x14ac:dyDescent="0.25"/>
-    <row r="183" s="5" customFormat="1" x14ac:dyDescent="0.25"/>
-    <row r="184" s="5" customFormat="1" x14ac:dyDescent="0.25"/>
-    <row r="185" s="5" customFormat="1" x14ac:dyDescent="0.25"/>
-    <row r="186" s="5" customFormat="1" x14ac:dyDescent="0.25"/>
-    <row r="187" s="5" customFormat="1" x14ac:dyDescent="0.25"/>
+      <c r="L45" s="83"/>
+      <c r="M45" s="83"/>
+      <c r="N45" s="83"/>
+      <c r="O45" s="83"/>
+      <c r="P45" s="83"/>
+    </row>
+    <row r="46" spans="1:16" s="5" customFormat="1" x14ac:dyDescent="0.3"/>
+    <row r="47" spans="1:16" s="5" customFormat="1" x14ac:dyDescent="0.3"/>
+    <row r="48" spans="1:16" s="5" customFormat="1" x14ac:dyDescent="0.3"/>
+    <row r="49" s="5" customFormat="1" x14ac:dyDescent="0.3"/>
+    <row r="50" s="5" customFormat="1" x14ac:dyDescent="0.3"/>
+    <row r="51" s="5" customFormat="1" x14ac:dyDescent="0.3"/>
+    <row r="52" s="5" customFormat="1" x14ac:dyDescent="0.3"/>
+    <row r="53" s="5" customFormat="1" x14ac:dyDescent="0.3"/>
+    <row r="54" s="5" customFormat="1" x14ac:dyDescent="0.3"/>
+    <row r="55" s="5" customFormat="1" x14ac:dyDescent="0.3"/>
+    <row r="56" s="5" customFormat="1" x14ac:dyDescent="0.3"/>
+    <row r="57" s="5" customFormat="1" x14ac:dyDescent="0.3"/>
+    <row r="58" s="5" customFormat="1" x14ac:dyDescent="0.3"/>
+    <row r="59" s="5" customFormat="1" x14ac:dyDescent="0.3"/>
+    <row r="60" s="5" customFormat="1" x14ac:dyDescent="0.3"/>
+    <row r="61" s="5" customFormat="1" x14ac:dyDescent="0.3"/>
+    <row r="62" s="5" customFormat="1" x14ac:dyDescent="0.3"/>
+    <row r="63" s="5" customFormat="1" x14ac:dyDescent="0.3"/>
+    <row r="64" s="5" customFormat="1" x14ac:dyDescent="0.3"/>
+    <row r="65" s="5" customFormat="1" x14ac:dyDescent="0.3"/>
+    <row r="66" s="5" customFormat="1" x14ac:dyDescent="0.3"/>
+    <row r="67" s="5" customFormat="1" x14ac:dyDescent="0.3"/>
+    <row r="68" s="5" customFormat="1" x14ac:dyDescent="0.3"/>
+    <row r="69" s="5" customFormat="1" x14ac:dyDescent="0.3"/>
+    <row r="70" s="5" customFormat="1" x14ac:dyDescent="0.3"/>
+    <row r="71" s="5" customFormat="1" x14ac:dyDescent="0.3"/>
+    <row r="72" s="5" customFormat="1" x14ac:dyDescent="0.3"/>
+    <row r="73" s="5" customFormat="1" x14ac:dyDescent="0.3"/>
+    <row r="74" s="5" customFormat="1" x14ac:dyDescent="0.3"/>
+    <row r="75" s="5" customFormat="1" x14ac:dyDescent="0.3"/>
+    <row r="76" s="5" customFormat="1" x14ac:dyDescent="0.3"/>
+    <row r="77" s="5" customFormat="1" x14ac:dyDescent="0.3"/>
+    <row r="78" s="5" customFormat="1" x14ac:dyDescent="0.3"/>
+    <row r="79" s="5" customFormat="1" x14ac:dyDescent="0.3"/>
+    <row r="80" s="5" customFormat="1" x14ac:dyDescent="0.3"/>
+    <row r="81" s="5" customFormat="1" x14ac:dyDescent="0.3"/>
+    <row r="82" s="5" customFormat="1" x14ac:dyDescent="0.3"/>
+    <row r="83" s="5" customFormat="1" x14ac:dyDescent="0.3"/>
+    <row r="84" s="5" customFormat="1" x14ac:dyDescent="0.3"/>
+    <row r="85" s="5" customFormat="1" x14ac:dyDescent="0.3"/>
+    <row r="86" s="5" customFormat="1" x14ac:dyDescent="0.3"/>
+    <row r="87" s="5" customFormat="1" x14ac:dyDescent="0.3"/>
+    <row r="88" s="5" customFormat="1" x14ac:dyDescent="0.3"/>
+    <row r="89" s="5" customFormat="1" x14ac:dyDescent="0.3"/>
+    <row r="90" s="5" customFormat="1" x14ac:dyDescent="0.3"/>
+    <row r="91" s="5" customFormat="1" x14ac:dyDescent="0.3"/>
+    <row r="92" s="5" customFormat="1" x14ac:dyDescent="0.3"/>
+    <row r="93" s="5" customFormat="1" x14ac:dyDescent="0.3"/>
+    <row r="94" s="5" customFormat="1" x14ac:dyDescent="0.3"/>
+    <row r="95" s="5" customFormat="1" x14ac:dyDescent="0.3"/>
+    <row r="96" s="5" customFormat="1" x14ac:dyDescent="0.3"/>
+    <row r="97" s="5" customFormat="1" x14ac:dyDescent="0.3"/>
+    <row r="98" s="5" customFormat="1" x14ac:dyDescent="0.3"/>
+    <row r="99" s="5" customFormat="1" x14ac:dyDescent="0.3"/>
+    <row r="100" s="5" customFormat="1" x14ac:dyDescent="0.3"/>
+    <row r="101" s="5" customFormat="1" x14ac:dyDescent="0.3"/>
+    <row r="102" s="5" customFormat="1" x14ac:dyDescent="0.3"/>
+    <row r="103" s="5" customFormat="1" x14ac:dyDescent="0.3"/>
+    <row r="104" s="5" customFormat="1" x14ac:dyDescent="0.3"/>
+    <row r="105" s="5" customFormat="1" x14ac:dyDescent="0.3"/>
+    <row r="106" s="5" customFormat="1" x14ac:dyDescent="0.3"/>
+    <row r="107" s="5" customFormat="1" x14ac:dyDescent="0.3"/>
+    <row r="108" s="5" customFormat="1" x14ac:dyDescent="0.3"/>
+    <row r="109" s="5" customFormat="1" x14ac:dyDescent="0.3"/>
+    <row r="110" s="5" customFormat="1" x14ac:dyDescent="0.3"/>
+    <row r="111" s="5" customFormat="1" x14ac:dyDescent="0.3"/>
+    <row r="112" s="5" customFormat="1" x14ac:dyDescent="0.3"/>
+    <row r="113" s="5" customFormat="1" x14ac:dyDescent="0.3"/>
+    <row r="114" s="5" customFormat="1" x14ac:dyDescent="0.3"/>
+    <row r="115" s="5" customFormat="1" x14ac:dyDescent="0.3"/>
+    <row r="116" s="5" customFormat="1" x14ac:dyDescent="0.3"/>
+    <row r="117" s="5" customFormat="1" x14ac:dyDescent="0.3"/>
+    <row r="118" s="5" customFormat="1" x14ac:dyDescent="0.3"/>
+    <row r="119" s="5" customFormat="1" x14ac:dyDescent="0.3"/>
+    <row r="120" s="5" customFormat="1" x14ac:dyDescent="0.3"/>
+    <row r="121" s="5" customFormat="1" x14ac:dyDescent="0.3"/>
+    <row r="122" s="5" customFormat="1" x14ac:dyDescent="0.3"/>
+    <row r="123" s="5" customFormat="1" x14ac:dyDescent="0.3"/>
+    <row r="124" s="5" customFormat="1" x14ac:dyDescent="0.3"/>
+    <row r="125" s="5" customFormat="1" x14ac:dyDescent="0.3"/>
+    <row r="126" s="5" customFormat="1" x14ac:dyDescent="0.3"/>
+    <row r="127" s="5" customFormat="1" x14ac:dyDescent="0.3"/>
+    <row r="128" s="5" customFormat="1" x14ac:dyDescent="0.3"/>
+    <row r="129" s="5" customFormat="1" x14ac:dyDescent="0.3"/>
+    <row r="130" s="5" customFormat="1" x14ac:dyDescent="0.3"/>
+    <row r="131" s="5" customFormat="1" x14ac:dyDescent="0.3"/>
+    <row r="132" s="5" customFormat="1" x14ac:dyDescent="0.3"/>
+    <row r="133" s="5" customFormat="1" x14ac:dyDescent="0.3"/>
+    <row r="134" s="5" customFormat="1" x14ac:dyDescent="0.3"/>
+    <row r="135" s="5" customFormat="1" x14ac:dyDescent="0.3"/>
+    <row r="136" s="5" customFormat="1" x14ac:dyDescent="0.3"/>
+    <row r="137" s="5" customFormat="1" x14ac:dyDescent="0.3"/>
+    <row r="138" s="5" customFormat="1" x14ac:dyDescent="0.3"/>
+    <row r="139" s="5" customFormat="1" x14ac:dyDescent="0.3"/>
+    <row r="140" s="5" customFormat="1" x14ac:dyDescent="0.3"/>
+    <row r="141" s="5" customFormat="1" x14ac:dyDescent="0.3"/>
+    <row r="142" s="5" customFormat="1" x14ac:dyDescent="0.3"/>
+    <row r="143" s="5" customFormat="1" x14ac:dyDescent="0.3"/>
+    <row r="144" s="5" customFormat="1" x14ac:dyDescent="0.3"/>
+    <row r="145" s="5" customFormat="1" x14ac:dyDescent="0.3"/>
+    <row r="146" s="5" customFormat="1" x14ac:dyDescent="0.3"/>
+    <row r="147" s="5" customFormat="1" x14ac:dyDescent="0.3"/>
+    <row r="148" s="5" customFormat="1" x14ac:dyDescent="0.3"/>
+    <row r="149" s="5" customFormat="1" x14ac:dyDescent="0.3"/>
+    <row r="150" s="5" customFormat="1" x14ac:dyDescent="0.3"/>
+    <row r="151" s="5" customFormat="1" x14ac:dyDescent="0.3"/>
+    <row r="152" s="5" customFormat="1" x14ac:dyDescent="0.3"/>
+    <row r="153" s="5" customFormat="1" x14ac:dyDescent="0.3"/>
+    <row r="154" s="5" customFormat="1" x14ac:dyDescent="0.3"/>
+    <row r="155" s="5" customFormat="1" x14ac:dyDescent="0.3"/>
+    <row r="156" s="5" customFormat="1" x14ac:dyDescent="0.3"/>
+    <row r="157" s="5" customFormat="1" x14ac:dyDescent="0.3"/>
+    <row r="158" s="5" customFormat="1" x14ac:dyDescent="0.3"/>
+    <row r="159" s="5" customFormat="1" x14ac:dyDescent="0.3"/>
+    <row r="160" s="5" customFormat="1" x14ac:dyDescent="0.3"/>
+    <row r="161" s="5" customFormat="1" x14ac:dyDescent="0.3"/>
+    <row r="162" s="5" customFormat="1" x14ac:dyDescent="0.3"/>
+    <row r="163" s="5" customFormat="1" x14ac:dyDescent="0.3"/>
+    <row r="164" s="5" customFormat="1" x14ac:dyDescent="0.3"/>
+    <row r="165" s="5" customFormat="1" x14ac:dyDescent="0.3"/>
+    <row r="166" s="5" customFormat="1" x14ac:dyDescent="0.3"/>
+    <row r="167" s="5" customFormat="1" x14ac:dyDescent="0.3"/>
+    <row r="168" s="5" customFormat="1" x14ac:dyDescent="0.3"/>
+    <row r="169" s="5" customFormat="1" x14ac:dyDescent="0.3"/>
+    <row r="170" s="5" customFormat="1" x14ac:dyDescent="0.3"/>
+    <row r="171" s="5" customFormat="1" x14ac:dyDescent="0.3"/>
+    <row r="172" s="5" customFormat="1" x14ac:dyDescent="0.3"/>
+    <row r="173" s="5" customFormat="1" x14ac:dyDescent="0.3"/>
+    <row r="174" s="5" customFormat="1" x14ac:dyDescent="0.3"/>
+    <row r="175" s="5" customFormat="1" x14ac:dyDescent="0.3"/>
+    <row r="176" s="5" customFormat="1" x14ac:dyDescent="0.3"/>
+    <row r="177" s="5" customFormat="1" x14ac:dyDescent="0.3"/>
+    <row r="178" s="5" customFormat="1" x14ac:dyDescent="0.3"/>
+    <row r="179" s="5" customFormat="1" x14ac:dyDescent="0.3"/>
+    <row r="180" s="5" customFormat="1" x14ac:dyDescent="0.3"/>
+    <row r="181" s="5" customFormat="1" x14ac:dyDescent="0.3"/>
+    <row r="182" s="5" customFormat="1" x14ac:dyDescent="0.3"/>
+    <row r="183" s="5" customFormat="1" x14ac:dyDescent="0.3"/>
+    <row r="184" s="5" customFormat="1" x14ac:dyDescent="0.3"/>
+    <row r="185" s="5" customFormat="1" x14ac:dyDescent="0.3"/>
+    <row r="186" s="5" customFormat="1" x14ac:dyDescent="0.3"/>
+    <row r="187" s="5" customFormat="1" x14ac:dyDescent="0.3"/>
   </sheetData>
   <mergeCells count="41">
+    <mergeCell ref="I2:J2"/>
+    <mergeCell ref="K2:L2"/>
+    <mergeCell ref="B3:C3"/>
+    <mergeCell ref="D3:E3"/>
+    <mergeCell ref="I3:J3"/>
+    <mergeCell ref="K3:L3"/>
+    <mergeCell ref="B11:C11"/>
+    <mergeCell ref="D11:E11"/>
+    <mergeCell ref="H18:J18"/>
+    <mergeCell ref="K18:L18"/>
+    <mergeCell ref="B18:C18"/>
+    <mergeCell ref="D18:E18"/>
+    <mergeCell ref="H14:L14"/>
+    <mergeCell ref="H15:L15"/>
+    <mergeCell ref="H19:J19"/>
+    <mergeCell ref="K19:L19"/>
+    <mergeCell ref="H20:J20"/>
+    <mergeCell ref="K20:L20"/>
+    <mergeCell ref="H21:J21"/>
+    <mergeCell ref="K21:L21"/>
+    <mergeCell ref="K22:L22"/>
+    <mergeCell ref="H23:J23"/>
+    <mergeCell ref="K23:L23"/>
+    <mergeCell ref="H24:J24"/>
+    <mergeCell ref="K24:L24"/>
     <mergeCell ref="C28:E28"/>
     <mergeCell ref="F28:G28"/>
     <mergeCell ref="M37:P37"/>
@@ -5928,31 +6007,6 @@
     <mergeCell ref="M17:N17"/>
     <mergeCell ref="H17:L17"/>
     <mergeCell ref="H22:J22"/>
-    <mergeCell ref="K22:L22"/>
-    <mergeCell ref="H23:J23"/>
-    <mergeCell ref="K23:L23"/>
-    <mergeCell ref="H24:J24"/>
-    <mergeCell ref="K24:L24"/>
-    <mergeCell ref="H19:J19"/>
-    <mergeCell ref="K19:L19"/>
-    <mergeCell ref="H20:J20"/>
-    <mergeCell ref="K20:L20"/>
-    <mergeCell ref="H21:J21"/>
-    <mergeCell ref="K21:L21"/>
-    <mergeCell ref="B11:C11"/>
-    <mergeCell ref="D11:E11"/>
-    <mergeCell ref="H18:J18"/>
-    <mergeCell ref="K18:L18"/>
-    <mergeCell ref="B18:C18"/>
-    <mergeCell ref="D18:E18"/>
-    <mergeCell ref="H14:L14"/>
-    <mergeCell ref="H15:L15"/>
-    <mergeCell ref="I2:J2"/>
-    <mergeCell ref="K2:L2"/>
-    <mergeCell ref="B3:C3"/>
-    <mergeCell ref="D3:E3"/>
-    <mergeCell ref="I3:J3"/>
-    <mergeCell ref="K3:L3"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <drawing r:id="rId1"/>
@@ -5968,55 +6022,55 @@
       <selection activeCell="I13" sqref="I13"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr baseColWidth="10" defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <cols>
     <col min="1" max="1" width="7" customWidth="1"/>
-    <col min="2" max="4" width="8.42578125" customWidth="1"/>
-    <col min="5" max="6" width="7.5703125" customWidth="1"/>
+    <col min="2" max="4" width="8.44140625" customWidth="1"/>
+    <col min="5" max="6" width="7.5546875" customWidth="1"/>
     <col min="7" max="8" width="10" customWidth="1"/>
-    <col min="9" max="9" width="5.28515625" customWidth="1"/>
-    <col min="10" max="10" width="10.7109375" customWidth="1"/>
-    <col min="11" max="11" width="9.5703125" customWidth="1"/>
-    <col min="12" max="12" width="10.5703125" customWidth="1"/>
-    <col min="13" max="13" width="4.140625" customWidth="1"/>
+    <col min="9" max="9" width="5.33203125" customWidth="1"/>
+    <col min="10" max="10" width="10.6640625" customWidth="1"/>
+    <col min="11" max="11" width="9.5546875" customWidth="1"/>
+    <col min="12" max="12" width="10.5546875" customWidth="1"/>
+    <col min="13" max="13" width="4.109375" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="2:17" ht="15.75" thickBot="1" x14ac:dyDescent="0.3"/>
-    <row r="2" spans="2:17" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="B2" s="91" t="s">
+    <row r="1" spans="2:17" ht="15" thickBot="1" x14ac:dyDescent="0.35"/>
+    <row r="2" spans="2:17" ht="15" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="B2" s="87" t="s">
         <v>82</v>
       </c>
-      <c r="C2" s="93"/>
-      <c r="D2" s="93"/>
-      <c r="E2" s="93"/>
-      <c r="F2" s="92"/>
-      <c r="G2" s="91" t="s">
+      <c r="C2" s="89"/>
+      <c r="D2" s="89"/>
+      <c r="E2" s="89"/>
+      <c r="F2" s="88"/>
+      <c r="G2" s="87" t="s">
         <v>44</v>
       </c>
-      <c r="H2" s="92"/>
+      <c r="H2" s="88"/>
       <c r="J2" s="50" t="s">
         <v>79</v>
       </c>
-      <c r="K2" s="91" t="s">
+      <c r="K2" s="87" t="s">
         <v>81</v>
       </c>
-      <c r="L2" s="92"/>
+      <c r="L2" s="88"/>
       <c r="M2" s="29"/>
       <c r="N2" s="100" t="s">
         <v>44</v>
       </c>
       <c r="O2" s="101"/>
     </row>
-    <row r="3" spans="2:17" x14ac:dyDescent="0.25">
-      <c r="B3" s="81" t="s">
+    <row r="3" spans="2:17" x14ac:dyDescent="0.3">
+      <c r="B3" s="94" t="s">
         <v>24</v>
       </c>
-      <c r="C3" s="82"/>
-      <c r="D3" s="82"/>
-      <c r="E3" s="82" t="s">
+      <c r="C3" s="95"/>
+      <c r="D3" s="95"/>
+      <c r="E3" s="95" t="s">
         <v>35</v>
       </c>
-      <c r="F3" s="82"/>
+      <c r="F3" s="95"/>
       <c r="G3" s="10" t="s">
         <v>25</v>
       </c>
@@ -6038,16 +6092,16 @@
         <v>58</v>
       </c>
     </row>
-    <row r="4" spans="2:17" x14ac:dyDescent="0.25">
-      <c r="B4" s="83" t="s">
+    <row r="4" spans="2:17" x14ac:dyDescent="0.3">
+      <c r="B4" s="84" t="s">
         <v>30</v>
       </c>
-      <c r="C4" s="84"/>
-      <c r="D4" s="84"/>
-      <c r="E4" s="84" t="s">
+      <c r="C4" s="81"/>
+      <c r="D4" s="81"/>
+      <c r="E4" s="81" t="s">
         <v>31</v>
       </c>
-      <c r="F4" s="84"/>
+      <c r="F4" s="81"/>
       <c r="G4" s="11" t="s">
         <v>39</v>
       </c>
@@ -6069,16 +6123,16 @@
         <v>60</v>
       </c>
     </row>
-    <row r="5" spans="2:17" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="B5" s="83" t="s">
+    <row r="5" spans="2:17" ht="15" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="B5" s="84" t="s">
         <v>32</v>
       </c>
-      <c r="C5" s="84"/>
-      <c r="D5" s="84"/>
-      <c r="E5" s="84" t="s">
+      <c r="C5" s="81"/>
+      <c r="D5" s="81"/>
+      <c r="E5" s="81" t="s">
         <v>33</v>
       </c>
-      <c r="F5" s="84"/>
+      <c r="F5" s="81"/>
       <c r="G5" s="11" t="s">
         <v>37</v>
       </c>
@@ -6099,16 +6153,16 @@
       </c>
       <c r="Q5" s="70"/>
     </row>
-    <row r="6" spans="2:17" x14ac:dyDescent="0.25">
-      <c r="B6" s="83" t="s">
+    <row r="6" spans="2:17" x14ac:dyDescent="0.3">
+      <c r="B6" s="84" t="s">
         <v>43</v>
       </c>
-      <c r="C6" s="84"/>
-      <c r="D6" s="84"/>
-      <c r="E6" s="84" t="s">
+      <c r="C6" s="81"/>
+      <c r="D6" s="81"/>
+      <c r="E6" s="81" t="s">
         <v>36</v>
       </c>
-      <c r="F6" s="84"/>
+      <c r="F6" s="81"/>
       <c r="G6" s="11" t="s">
         <v>38</v>
       </c>
@@ -6117,16 +6171,16 @@
       </c>
       <c r="Q6" s="70"/>
     </row>
-    <row r="7" spans="2:17" x14ac:dyDescent="0.25">
-      <c r="B7" s="94" t="s">
+    <row r="7" spans="2:17" x14ac:dyDescent="0.3">
+      <c r="B7" s="90" t="s">
         <v>27</v>
       </c>
-      <c r="C7" s="95"/>
-      <c r="D7" s="86"/>
-      <c r="E7" s="85" t="s">
+      <c r="C7" s="91"/>
+      <c r="D7" s="92"/>
+      <c r="E7" s="93" t="s">
         <v>67</v>
       </c>
-      <c r="F7" s="86"/>
+      <c r="F7" s="92"/>
       <c r="G7" s="11" t="s">
         <v>40</v>
       </c>
@@ -6134,16 +6188,16 @@
         <v>42</v>
       </c>
     </row>
-    <row r="8" spans="2:17" x14ac:dyDescent="0.25">
-      <c r="B8" s="83" t="s">
+    <row r="8" spans="2:17" x14ac:dyDescent="0.3">
+      <c r="B8" s="84" t="s">
         <v>28</v>
       </c>
-      <c r="C8" s="84"/>
-      <c r="D8" s="84"/>
-      <c r="E8" s="84" t="s">
+      <c r="C8" s="81"/>
+      <c r="D8" s="81"/>
+      <c r="E8" s="81" t="s">
         <v>26</v>
       </c>
-      <c r="F8" s="84"/>
+      <c r="F8" s="81"/>
       <c r="G8" s="11" t="s">
         <v>41</v>
       </c>
@@ -6163,12 +6217,12 @@
       </c>
       <c r="O8" s="96"/>
     </row>
-    <row r="9" spans="2:17" x14ac:dyDescent="0.25">
-      <c r="B9" s="83"/>
-      <c r="C9" s="84"/>
-      <c r="D9" s="84"/>
-      <c r="E9" s="84"/>
-      <c r="F9" s="84"/>
+    <row r="9" spans="2:17" x14ac:dyDescent="0.3">
+      <c r="B9" s="84"/>
+      <c r="C9" s="81"/>
+      <c r="D9" s="81"/>
+      <c r="E9" s="81"/>
+      <c r="F9" s="81"/>
       <c r="G9" s="9"/>
       <c r="H9" s="12"/>
       <c r="J9" s="65"/>
@@ -6183,12 +6237,12 @@
         <v>58</v>
       </c>
     </row>
-    <row r="10" spans="2:17" x14ac:dyDescent="0.25">
-      <c r="B10" s="83"/>
-      <c r="C10" s="84"/>
-      <c r="D10" s="84"/>
-      <c r="E10" s="84"/>
-      <c r="F10" s="84"/>
+    <row r="10" spans="2:17" x14ac:dyDescent="0.3">
+      <c r="B10" s="84"/>
+      <c r="C10" s="81"/>
+      <c r="D10" s="81"/>
+      <c r="E10" s="81"/>
+      <c r="F10" s="81"/>
       <c r="G10" s="9"/>
       <c r="H10" s="12"/>
       <c r="J10" s="65"/>
@@ -6205,16 +6259,16 @@
         <v>89</v>
       </c>
     </row>
-    <row r="11" spans="2:17" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="B11" s="89" t="s">
+    <row r="11" spans="2:17" ht="15" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="B11" s="85" t="s">
         <v>45</v>
       </c>
-      <c r="C11" s="90"/>
-      <c r="D11" s="90"/>
-      <c r="E11" s="90" t="s">
+      <c r="C11" s="86"/>
+      <c r="D11" s="86"/>
+      <c r="E11" s="86" t="s">
         <v>46</v>
       </c>
-      <c r="F11" s="90"/>
+      <c r="F11" s="86"/>
       <c r="G11" s="15" t="s">
         <v>47</v>
       </c>
@@ -6233,7 +6287,7 @@
         <v>58</v>
       </c>
     </row>
-    <row r="12" spans="2:17" x14ac:dyDescent="0.25">
+    <row r="12" spans="2:17" x14ac:dyDescent="0.3">
       <c r="J12" s="65"/>
       <c r="K12" s="1" t="s">
         <v>29</v>
@@ -6246,7 +6300,7 @@
         <v>58</v>
       </c>
     </row>
-    <row r="13" spans="2:17" x14ac:dyDescent="0.25">
+    <row r="13" spans="2:17" x14ac:dyDescent="0.3">
       <c r="J13" s="65"/>
       <c r="K13" s="1" t="s">
         <v>26</v>
@@ -6261,15 +6315,6 @@
     </row>
   </sheetData>
   <mergeCells count="25">
-    <mergeCell ref="E6:F6"/>
-    <mergeCell ref="B7:D7"/>
-    <mergeCell ref="E7:F7"/>
-    <mergeCell ref="B2:F2"/>
-    <mergeCell ref="G2:H2"/>
-    <mergeCell ref="B3:D3"/>
-    <mergeCell ref="E3:F3"/>
-    <mergeCell ref="B4:D4"/>
-    <mergeCell ref="E4:F4"/>
     <mergeCell ref="K8:L8"/>
     <mergeCell ref="N8:O8"/>
     <mergeCell ref="J3:J5"/>
@@ -6286,6 +6331,15 @@
     <mergeCell ref="B5:D5"/>
     <mergeCell ref="E5:F5"/>
     <mergeCell ref="B6:D6"/>
+    <mergeCell ref="E6:F6"/>
+    <mergeCell ref="B7:D7"/>
+    <mergeCell ref="E7:F7"/>
+    <mergeCell ref="B2:F2"/>
+    <mergeCell ref="G2:H2"/>
+    <mergeCell ref="B3:D3"/>
+    <mergeCell ref="E3:F3"/>
+    <mergeCell ref="B4:D4"/>
+    <mergeCell ref="E4:F4"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup paperSize="9" orientation="portrait" r:id="rId1"/>
@@ -6301,18 +6355,18 @@
       <selection activeCell="B12" sqref="B12"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr baseColWidth="10" defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <cols>
-    <col min="1" max="1" width="11.42578125" style="46"/>
-    <col min="4" max="5" width="11.42578125" style="46"/>
-    <col min="6" max="6" width="3.7109375" customWidth="1"/>
+    <col min="1" max="1" width="11.44140625" style="46"/>
+    <col min="4" max="5" width="11.44140625" style="46"/>
+    <col min="6" max="6" width="3.6640625" customWidth="1"/>
     <col min="7" max="7" width="20" customWidth="1"/>
-    <col min="9" max="9" width="20.140625" customWidth="1"/>
-    <col min="12" max="12" width="10.28515625" customWidth="1"/>
+    <col min="9" max="9" width="20.109375" customWidth="1"/>
+    <col min="12" max="12" width="10.33203125" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:12" ht="15.75" thickBot="1" x14ac:dyDescent="0.3"/>
-    <row r="2" spans="1:12" ht="19.5" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="1" spans="1:12" ht="15" thickBot="1" x14ac:dyDescent="0.35"/>
+    <row r="2" spans="1:12" ht="18.600000000000001" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A2" s="102" t="s">
         <v>87</v>
       </c>
@@ -6323,13 +6377,13 @@
       <c r="F2" s="103"/>
       <c r="G2" s="104"/>
     </row>
-    <row r="3" spans="1:12" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="3" spans="1:12" ht="15" thickBot="1" x14ac:dyDescent="0.35">
       <c r="B3" s="46"/>
       <c r="C3" s="46"/>
       <c r="F3" s="46"/>
       <c r="G3" s="46"/>
     </row>
-    <row r="4" spans="1:12" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="4" spans="1:12" ht="15" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A4" s="61" t="s">
         <v>83</v>
       </c>
@@ -6349,7 +6403,7 @@
         <v>86</v>
       </c>
     </row>
-    <row r="5" spans="1:12" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="5" spans="1:12" ht="15" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A5" s="1">
         <v>0</v>
       </c>
@@ -6370,16 +6424,16 @@
       <c r="G5" s="63" t="s">
         <v>88</v>
       </c>
-      <c r="I5" s="91" t="s">
+      <c r="I5" s="87" t="s">
         <v>82</v>
       </c>
-      <c r="J5" s="93"/>
-      <c r="K5" s="91" t="s">
+      <c r="J5" s="89"/>
+      <c r="K5" s="87" t="s">
         <v>44</v>
       </c>
-      <c r="L5" s="92"/>
-    </row>
-    <row r="6" spans="1:12" x14ac:dyDescent="0.25">
+      <c r="L5" s="88"/>
+    </row>
+    <row r="6" spans="1:12" x14ac:dyDescent="0.3">
       <c r="A6" s="1">
         <f>A5+1</f>
         <v>1</v>
@@ -6411,7 +6465,7 @@
         <v>34</v>
       </c>
     </row>
-    <row r="7" spans="1:12" x14ac:dyDescent="0.25">
+    <row r="7" spans="1:12" x14ac:dyDescent="0.3">
       <c r="A7" s="1">
         <f t="shared" ref="A7:A24" si="2">A6+1</f>
         <v>2</v>
@@ -6443,7 +6497,7 @@
         <v>42</v>
       </c>
     </row>
-    <row r="8" spans="1:12" x14ac:dyDescent="0.25">
+    <row r="8" spans="1:12" x14ac:dyDescent="0.3">
       <c r="A8" s="1">
         <f t="shared" si="2"/>
         <v>3</v>
@@ -6475,7 +6529,7 @@
         <v>8</v>
       </c>
     </row>
-    <row r="9" spans="1:12" x14ac:dyDescent="0.25">
+    <row r="9" spans="1:12" x14ac:dyDescent="0.3">
       <c r="A9" s="1">
         <f t="shared" si="2"/>
         <v>4</v>
@@ -6507,7 +6561,7 @@
         <v>8</v>
       </c>
     </row>
-    <row r="10" spans="1:12" x14ac:dyDescent="0.25">
+    <row r="10" spans="1:12" x14ac:dyDescent="0.3">
       <c r="A10" s="1">
         <f t="shared" si="2"/>
         <v>5</v>
@@ -6539,7 +6593,7 @@
         <v>42</v>
       </c>
     </row>
-    <row r="11" spans="1:12" x14ac:dyDescent="0.25">
+    <row r="11" spans="1:12" x14ac:dyDescent="0.3">
       <c r="A11" s="1">
         <f t="shared" si="2"/>
         <v>6</v>
@@ -6571,7 +6625,7 @@
         <v>42</v>
       </c>
     </row>
-    <row r="12" spans="1:12" x14ac:dyDescent="0.25">
+    <row r="12" spans="1:12" x14ac:dyDescent="0.3">
       <c r="A12" s="1">
         <f t="shared" si="2"/>
         <v>7</v>
@@ -6595,7 +6649,7 @@
       <c r="K12" s="9"/>
       <c r="L12" s="12"/>
     </row>
-    <row r="13" spans="1:12" x14ac:dyDescent="0.25">
+    <row r="13" spans="1:12" x14ac:dyDescent="0.3">
       <c r="A13" s="1">
         <f t="shared" si="2"/>
         <v>8</v>
@@ -6617,7 +6671,7 @@
       <c r="K13" s="9"/>
       <c r="L13" s="12"/>
     </row>
-    <row r="14" spans="1:12" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="14" spans="1:12" ht="15" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A14" s="1">
         <f t="shared" si="2"/>
         <v>9</v>
@@ -6647,7 +6701,7 @@
         <v>42</v>
       </c>
     </row>
-    <row r="15" spans="1:12" x14ac:dyDescent="0.25">
+    <row r="15" spans="1:12" x14ac:dyDescent="0.3">
       <c r="A15" s="1">
         <f t="shared" si="2"/>
         <v>10</v>
@@ -6665,7 +6719,7 @@
         <v>00000</v>
       </c>
     </row>
-    <row r="16" spans="1:12" x14ac:dyDescent="0.25">
+    <row r="16" spans="1:12" x14ac:dyDescent="0.3">
       <c r="A16" s="1">
         <f t="shared" si="2"/>
         <v>11</v>
@@ -6683,7 +6737,7 @@
         <v>00000</v>
       </c>
     </row>
-    <row r="17" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="17" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A17" s="1">
         <f t="shared" si="2"/>
         <v>12</v>
@@ -6701,7 +6755,7 @@
         <v>00000</v>
       </c>
     </row>
-    <row r="18" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="18" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A18" s="1">
         <f t="shared" si="2"/>
         <v>13</v>
@@ -6719,7 +6773,7 @@
         <v>00000</v>
       </c>
     </row>
-    <row r="19" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="19" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A19" s="1">
         <f t="shared" si="2"/>
         <v>14</v>
@@ -6737,7 +6791,7 @@
         <v>00000</v>
       </c>
     </row>
-    <row r="20" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="20" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A20" s="1">
         <f t="shared" si="2"/>
         <v>15</v>
@@ -6755,7 +6809,7 @@
         <v>00000</v>
       </c>
     </row>
-    <row r="21" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="21" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A21" s="1">
         <f t="shared" si="2"/>
         <v>16</v>
@@ -6773,7 +6827,7 @@
         <v>00000</v>
       </c>
     </row>
-    <row r="22" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="22" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A22" s="1">
         <f t="shared" si="2"/>
         <v>17</v>
@@ -6791,7 +6845,7 @@
         <v>00000</v>
       </c>
     </row>
-    <row r="23" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="23" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A23" s="1">
         <f t="shared" si="2"/>
         <v>18</v>
@@ -6809,7 +6863,7 @@
         <v>00000</v>
       </c>
     </row>
-    <row r="24" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="24" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A24" s="1">
         <f t="shared" si="2"/>
         <v>19</v>
@@ -6849,15 +6903,15 @@
             <anchor moveWithCells="1">
               <from>
                 <xdr:col>6</xdr:col>
-                <xdr:colOff>9525</xdr:colOff>
+                <xdr:colOff>7620</xdr:colOff>
                 <xdr:row>5</xdr:row>
-                <xdr:rowOff>85725</xdr:rowOff>
+                <xdr:rowOff>83820</xdr:rowOff>
               </from>
               <to>
-                <xdr:col>7</xdr:col>
-                <xdr:colOff>28575</xdr:colOff>
+                <xdr:col>6</xdr:col>
+                <xdr:colOff>1356360</xdr:colOff>
                 <xdr:row>7</xdr:row>
-                <xdr:rowOff>47625</xdr:rowOff>
+                <xdr:rowOff>60960</xdr:rowOff>
               </to>
             </anchor>
           </controlPr>
@@ -6880,7 +6934,7 @@
       <selection activeCell="G10" sqref="G10"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr baseColWidth="10" defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <sheetData/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>

</xml_diff>